<commit_message>
minor edit to the spreadsheet
</commit_message>
<xml_diff>
--- a/Data/flow/NO3-N Loss.xlsx
+++ b/Data/flow/NO3-N Loss.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17571"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gio\Documents\GitHub\CSCAP\Sustainable_Corn_Paper\Data\flow\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gio\Documents\GitHub\CSCAP\Sustainable_Corn_Paper\Data\flow\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11985" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11985" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sites" sheetId="1" r:id="rId1"/>
@@ -21,12 +21,12 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Data!$A$1:$G$248</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">rotations!$A$1:$H$63</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">SERF!$A$16:$E$47</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">SERF!$S$16:$W$47</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sites!$A$2:$D$2</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
   <pivotCaches>
-    <pivotCache cacheId="34" r:id="rId6"/>
+    <pivotCache cacheId="0" r:id="rId6"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -735,13 +735,13 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0.000_);_(* \(#,##0.000\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -868,8 +868,46 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -897,6 +935,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -993,7 +1037,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -1145,10 +1189,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="18" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="19" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="18" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="21" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="22" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1171,7 +1238,7 @@
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Chighladze, Giorgi" refreshedDate="42748.437253819444" createdVersion="5" refreshedVersion="5" minRefreshableVersion="3" recordCount="30">
   <cacheSource type="worksheet">
-    <worksheetSource ref="I2:M32" sheet="SERF"/>
+    <worksheetSource ref="AA2:AE32" sheet="SERF"/>
   </cacheSource>
   <cacheFields count="5">
     <cacheField name="plot id" numFmtId="0">
@@ -1421,8 +1488,8 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable9" cacheId="34" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="O1:R8" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable9" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="AG1:AJ8" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField axis="axisRow" showAll="0">
       <items count="7">
@@ -2081,11 +2148,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S248"/>
+  <dimension ref="A1:J248"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="W6" sqref="W6"/>
+      <selection pane="bottomLeft" activeCell="L1" sqref="L1:S31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2100,7 +2167,7 @@
     <col min="14" max="16" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="14" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="14" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>21</v>
       </c>
@@ -2129,23 +2196,8 @@
         <v>217</v>
       </c>
       <c r="J1"/>
-      <c r="L1" s="63" t="s">
-        <v>218</v>
-      </c>
-      <c r="M1" s="63" t="s">
-        <v>48</v>
-      </c>
-      <c r="N1" s="63" t="s">
-        <v>225</v>
-      </c>
-      <c r="O1" s="14" t="s">
-        <v>226</v>
-      </c>
-      <c r="P1" s="14" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>4</v>
       </c>
@@ -2173,30 +2225,8 @@
       <c r="I2" s="12">
         <v>29.855460999999998</v>
       </c>
-      <c r="L2" t="s">
-        <v>219</v>
-      </c>
-      <c r="M2" s="17">
-        <v>2011</v>
-      </c>
-      <c r="N2" s="12">
-        <v>23.452044000000001</v>
-      </c>
-      <c r="O2" s="57">
-        <v>29.855460999999998</v>
-      </c>
-      <c r="P2" s="12">
-        <v>9.1240900000000007</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>228</v>
-      </c>
-      <c r="S2" s="64">
-        <f>(P2-N2)/P2</f>
-        <v>-1.570343343829357</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>4</v>
       </c>
@@ -2224,30 +2254,8 @@
       <c r="I3" s="12">
         <v>42.465522999999997</v>
       </c>
-      <c r="L3" t="s">
-        <v>219</v>
-      </c>
-      <c r="M3" s="17">
-        <v>2012</v>
-      </c>
-      <c r="N3" s="12">
-        <v>11.148345000000001</v>
-      </c>
-      <c r="O3" s="12">
-        <v>11.148345000000001</v>
-      </c>
-      <c r="P3" s="12">
-        <v>14.43534</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>228</v>
-      </c>
-      <c r="S3" s="64">
-        <f t="shared" ref="S3:S31" si="0">(P3-N3)/P3</f>
-        <v>0.22770471634197734</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>4</v>
       </c>
@@ -2275,30 +2283,8 @@
       <c r="I4" s="12">
         <v>11.357567</v>
       </c>
-      <c r="L4" t="s">
-        <v>219</v>
-      </c>
-      <c r="M4" s="17">
-        <v>2013</v>
-      </c>
-      <c r="N4" s="12">
-        <v>20.605733000000001</v>
-      </c>
-      <c r="O4" s="12">
-        <v>20.605730000000001</v>
-      </c>
-      <c r="P4" s="12">
-        <v>23.84834</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>228</v>
-      </c>
-      <c r="S4" s="64">
-        <f t="shared" si="0"/>
-        <v>0.13596782836876695</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>4</v>
       </c>
@@ -2326,30 +2312,8 @@
       <c r="I5" s="12">
         <v>10.164596</v>
       </c>
-      <c r="L5" t="s">
-        <v>219</v>
-      </c>
-      <c r="M5" s="17">
-        <v>2014</v>
-      </c>
-      <c r="N5" s="12">
-        <v>21.997187</v>
-      </c>
-      <c r="O5" s="12">
-        <v>21.997187</v>
-      </c>
-      <c r="P5" s="12">
-        <v>37.060639999999999</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>228</v>
-      </c>
-      <c r="S5" s="64">
-        <f t="shared" si="0"/>
-        <v>0.40645420586368719</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>4</v>
       </c>
@@ -2377,30 +2341,8 @@
       <c r="I6" s="12">
         <v>24.493995999999999</v>
       </c>
-      <c r="L6" t="s">
-        <v>219</v>
-      </c>
-      <c r="M6" s="17">
-        <v>2015</v>
-      </c>
-      <c r="N6" s="12">
-        <v>6.4732370000000001</v>
-      </c>
-      <c r="O6" s="12">
-        <v>6.4732370000000001</v>
-      </c>
-      <c r="P6" s="12">
-        <v>10.604950000000001</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>228</v>
-      </c>
-      <c r="S6" s="64">
-        <f t="shared" si="0"/>
-        <v>0.38960230835600357</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>4</v>
       </c>
@@ -2428,30 +2370,8 @@
       <c r="I7" s="12">
         <v>5.7327260000000004</v>
       </c>
-      <c r="L7" t="s">
-        <v>220</v>
-      </c>
-      <c r="M7" s="17">
-        <v>2011</v>
-      </c>
-      <c r="N7" s="12">
-        <v>30.218699000000001</v>
-      </c>
-      <c r="O7" s="57">
-        <v>42.465522999999997</v>
-      </c>
-      <c r="P7" s="12">
-        <v>30.164850000000001</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>230</v>
-      </c>
-      <c r="S7" s="64">
-        <f t="shared" si="0"/>
-        <v>-1.7851572277004391E-3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>4</v>
       </c>
@@ -2467,30 +2387,8 @@
       <c r="E8" s="56">
         <v>11.148345000000001</v>
       </c>
-      <c r="L8" t="s">
-        <v>220</v>
-      </c>
-      <c r="M8" s="17">
-        <v>2012</v>
-      </c>
-      <c r="N8" s="12">
-        <v>12.322573999999999</v>
-      </c>
-      <c r="O8" s="12">
-        <v>12.322573999999999</v>
-      </c>
-      <c r="P8" s="12">
-        <v>12.300599999999999</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>230</v>
-      </c>
-      <c r="S8" s="64">
-        <f t="shared" si="0"/>
-        <v>-1.7864169227517488E-3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>4</v>
       </c>
@@ -2506,30 +2404,8 @@
       <c r="E9" s="56">
         <v>12.322573999999999</v>
       </c>
-      <c r="L9" t="s">
-        <v>220</v>
-      </c>
-      <c r="M9" s="17">
-        <v>2013</v>
-      </c>
-      <c r="N9" s="12">
-        <v>32.226103000000002</v>
-      </c>
-      <c r="O9" s="12">
-        <v>32.226100000000002</v>
-      </c>
-      <c r="P9" s="12">
-        <v>32.168640000000003</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>230</v>
-      </c>
-      <c r="S9" s="64">
-        <f t="shared" si="0"/>
-        <v>-1.7863049230554503E-3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>4</v>
       </c>
@@ -2545,30 +2421,8 @@
       <c r="E10" s="56">
         <v>4.2925409999999999</v>
       </c>
-      <c r="L10" t="s">
-        <v>220</v>
-      </c>
-      <c r="M10" s="17">
-        <v>2014</v>
-      </c>
-      <c r="N10" s="12">
-        <v>59.143658000000002</v>
-      </c>
-      <c r="O10" s="12">
-        <v>59.143658000000002</v>
-      </c>
-      <c r="P10" s="12">
-        <v>59.038209999999999</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>230</v>
-      </c>
-      <c r="S10" s="64">
-        <f t="shared" si="0"/>
-        <v>-1.7860975121028E-3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
         <v>4</v>
       </c>
@@ -2584,30 +2438,8 @@
       <c r="E11" s="56">
         <v>5.9977010000000002</v>
       </c>
-      <c r="L11" t="s">
-        <v>220</v>
-      </c>
-      <c r="M11" s="17">
-        <v>2015</v>
-      </c>
-      <c r="N11" s="12">
-        <v>14.899464999999999</v>
-      </c>
-      <c r="O11" s="12">
-        <v>14.899558000000001</v>
-      </c>
-      <c r="P11" s="12">
-        <v>14.8729</v>
-      </c>
-      <c r="Q11" t="s">
-        <v>230</v>
-      </c>
-      <c r="S11" s="64">
-        <f t="shared" si="0"/>
-        <v>-1.7861345131077145E-3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
         <v>4</v>
       </c>
@@ -2623,30 +2455,8 @@
       <c r="E12" s="56">
         <v>7.7289409999999998</v>
       </c>
-      <c r="L12" t="s">
-        <v>221</v>
-      </c>
-      <c r="M12" s="17">
-        <v>2011</v>
-      </c>
-      <c r="N12" s="12">
-        <v>9.6991209999999999</v>
-      </c>
-      <c r="O12" s="57">
-        <v>11.357567</v>
-      </c>
-      <c r="P12" s="12">
-        <v>9.6818270000000002</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>229</v>
-      </c>
-      <c r="S12" s="64">
-        <f t="shared" si="0"/>
-        <v>-1.7862331148862398E-3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
         <v>4</v>
       </c>
@@ -2662,30 +2472,8 @@
       <c r="E13" s="56">
         <v>3.6994479999999998</v>
       </c>
-      <c r="L13" t="s">
-        <v>221</v>
-      </c>
-      <c r="M13" s="17">
-        <v>2012</v>
-      </c>
-      <c r="N13" s="12">
-        <v>4.2925409999999999</v>
-      </c>
-      <c r="O13" s="12">
-        <v>4.2925409999999999</v>
-      </c>
-      <c r="P13" s="12">
-        <v>4.2848879999999996</v>
-      </c>
-      <c r="Q13" t="s">
-        <v>229</v>
-      </c>
-      <c r="S13" s="64">
-        <f t="shared" si="0"/>
-        <v>-1.7860443493506375E-3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
         <v>4</v>
       </c>
@@ -2701,30 +2489,8 @@
       <c r="E14" s="56">
         <v>20.605730000000001</v>
       </c>
-      <c r="L14" t="s">
-        <v>221</v>
-      </c>
-      <c r="M14" s="17">
-        <v>2013</v>
-      </c>
-      <c r="N14" s="12">
-        <v>19.107282999999999</v>
-      </c>
-      <c r="O14" s="12">
-        <v>19.107279999999999</v>
-      </c>
-      <c r="P14" s="12">
-        <v>19.07321</v>
-      </c>
-      <c r="Q14" t="s">
-        <v>229</v>
-      </c>
-      <c r="S14" s="64">
-        <f t="shared" si="0"/>
-        <v>-1.7864323834320156E-3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
         <v>4</v>
       </c>
@@ -2740,30 +2506,8 @@
       <c r="E15" s="56">
         <v>32.226100000000002</v>
       </c>
-      <c r="L15" t="s">
-        <v>221</v>
-      </c>
-      <c r="M15" s="17">
-        <v>2014</v>
-      </c>
-      <c r="N15" s="12">
-        <v>6.4460639999999998</v>
-      </c>
-      <c r="O15" s="12">
-        <v>6.4460639999999998</v>
-      </c>
-      <c r="P15" s="12">
-        <v>6.434571</v>
-      </c>
-      <c r="Q15" t="s">
-        <v>229</v>
-      </c>
-      <c r="S15" s="64">
-        <f t="shared" si="0"/>
-        <v>-1.7861330615513845E-3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
         <v>4</v>
       </c>
@@ -2779,30 +2523,8 @@
       <c r="E16" s="56">
         <v>19.107279999999999</v>
       </c>
-      <c r="L16" t="s">
-        <v>221</v>
-      </c>
-      <c r="M16" s="17">
-        <v>2015</v>
-      </c>
-      <c r="N16" s="12">
-        <v>10.609299</v>
-      </c>
-      <c r="O16" s="12">
-        <v>10.612791</v>
-      </c>
-      <c r="P16" s="12">
-        <v>10.59038</v>
-      </c>
-      <c r="Q16" t="s">
-        <v>229</v>
-      </c>
-      <c r="S16" s="64">
-        <f t="shared" si="0"/>
-        <v>-1.7864325925982215E-3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
         <v>4</v>
       </c>
@@ -2818,30 +2540,8 @@
       <c r="E17" s="56">
         <v>20.81466</v>
       </c>
-      <c r="L17" t="s">
-        <v>222</v>
-      </c>
-      <c r="M17" s="17">
-        <v>2011</v>
-      </c>
-      <c r="N17" s="12">
-        <v>9.5850329999999992</v>
-      </c>
-      <c r="O17" s="57">
-        <v>10.164596</v>
-      </c>
-      <c r="P17" s="12">
-        <v>9.5679420000000004</v>
-      </c>
-      <c r="Q17" t="s">
-        <v>229</v>
-      </c>
-      <c r="S17" s="64">
-        <f t="shared" si="0"/>
-        <v>-1.7862775505954004E-3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
         <v>4</v>
       </c>
@@ -2857,30 +2557,8 @@
       <c r="E18" s="56">
         <v>36.2149</v>
       </c>
-      <c r="L18" t="s">
-        <v>222</v>
-      </c>
-      <c r="M18" s="17">
-        <v>2012</v>
-      </c>
-      <c r="N18" s="12">
-        <v>5.9977010000000002</v>
-      </c>
-      <c r="O18" s="12">
-        <v>5.9977010000000002</v>
-      </c>
-      <c r="P18" s="12">
-        <v>5.9870070000000002</v>
-      </c>
-      <c r="Q18" t="s">
-        <v>229</v>
-      </c>
-      <c r="S18" s="64">
-        <f t="shared" si="0"/>
-        <v>-1.7862013523618698E-3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
         <v>4</v>
       </c>
@@ -2896,30 +2574,8 @@
       <c r="E19" s="56">
         <v>16.269770000000001</v>
       </c>
-      <c r="L19" t="s">
-        <v>222</v>
-      </c>
-      <c r="M19" s="17">
-        <v>2013</v>
-      </c>
-      <c r="N19" s="12">
-        <v>20.814662999999999</v>
-      </c>
-      <c r="O19" s="12">
-        <v>20.81466</v>
-      </c>
-      <c r="P19" s="12">
-        <v>20.777550000000002</v>
-      </c>
-      <c r="Q19" t="s">
-        <v>229</v>
-      </c>
-      <c r="S19" s="64">
-        <f t="shared" si="0"/>
-        <v>-1.7862067471861674E-3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>4</v>
       </c>
@@ -2935,30 +2591,8 @@
       <c r="E20" s="56">
         <v>21.997187</v>
       </c>
-      <c r="L20" t="s">
-        <v>222</v>
-      </c>
-      <c r="M20" s="17">
-        <v>2014</v>
-      </c>
-      <c r="N20" s="12">
-        <v>15.617248999999999</v>
-      </c>
-      <c r="O20" s="12">
-        <v>15.617248999999999</v>
-      </c>
-      <c r="P20" s="12">
-        <v>15.589399999999999</v>
-      </c>
-      <c r="Q20" t="s">
-        <v>229</v>
-      </c>
-      <c r="S20" s="64">
-        <f t="shared" si="0"/>
-        <v>-1.7864061477670592E-3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
         <v>4</v>
       </c>
@@ -2974,30 +2608,8 @@
       <c r="E21" s="56">
         <v>59.143658000000002</v>
       </c>
-      <c r="L21" t="s">
-        <v>222</v>
-      </c>
-      <c r="M21" s="17">
-        <v>2015</v>
-      </c>
-      <c r="N21" s="12">
-        <v>9.9696359999999995</v>
-      </c>
-      <c r="O21" s="12">
-        <v>9.9698910000000005</v>
-      </c>
-      <c r="P21" s="12">
-        <v>9.9518599999999999</v>
-      </c>
-      <c r="Q21" t="s">
-        <v>229</v>
-      </c>
-      <c r="S21" s="64">
-        <f t="shared" si="0"/>
-        <v>-1.7861987608346148E-3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
         <v>4</v>
       </c>
@@ -3013,30 +2625,8 @@
       <c r="E22" s="56">
         <v>6.4460639999999998</v>
       </c>
-      <c r="L22" t="s">
-        <v>223</v>
-      </c>
-      <c r="M22" s="17">
-        <v>2011</v>
-      </c>
-      <c r="N22" s="12">
-        <v>19.045133</v>
-      </c>
-      <c r="O22" s="57">
-        <v>24.493995999999999</v>
-      </c>
-      <c r="P22" s="12">
-        <v>19.01118</v>
-      </c>
-      <c r="Q22" t="s">
-        <v>230</v>
-      </c>
-      <c r="S22" s="64">
-        <f t="shared" si="0"/>
-        <v>-1.7859491099447981E-3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
         <v>4</v>
       </c>
@@ -3052,27 +2642,8 @@
       <c r="E23" s="56">
         <v>15.617248999999999</v>
       </c>
-      <c r="L23" t="s">
-        <v>223</v>
-      </c>
-      <c r="M23" s="17">
-        <v>2012</v>
-      </c>
-      <c r="N23" s="12">
-        <v>7.7289409999999998</v>
-      </c>
-      <c r="O23" s="12">
-        <v>7.7289409999999998</v>
-      </c>
-      <c r="P23" s="12">
-        <v>5.0621119999999997E-5</v>
-      </c>
-      <c r="Q23" t="s">
-        <v>230</v>
-      </c>
-      <c r="S23" s="64"/>
-    </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
         <v>4</v>
       </c>
@@ -3088,30 +2659,8 @@
       <c r="E24" s="56">
         <v>55.974493000000002</v>
       </c>
-      <c r="L24" t="s">
-        <v>223</v>
-      </c>
-      <c r="M24" s="17">
-        <v>2013</v>
-      </c>
-      <c r="N24" s="12">
-        <v>36.214897000000001</v>
-      </c>
-      <c r="O24" s="12">
-        <v>36.2149</v>
-      </c>
-      <c r="P24" s="12">
-        <v>36.150329999999997</v>
-      </c>
-      <c r="Q24" t="s">
-        <v>230</v>
-      </c>
-      <c r="S24" s="64">
-        <f t="shared" si="0"/>
-        <v>-1.7860694494352838E-3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="11" t="s">
         <v>4</v>
       </c>
@@ -3127,30 +2676,8 @@
       <c r="E25" s="56">
         <v>13.206845</v>
       </c>
-      <c r="L25" t="s">
-        <v>223</v>
-      </c>
-      <c r="M25" s="17">
-        <v>2014</v>
-      </c>
-      <c r="N25" s="12">
-        <v>55.974493000000002</v>
-      </c>
-      <c r="O25" s="12">
-        <v>55.974493000000002</v>
-      </c>
-      <c r="P25" s="12">
-        <v>55.874690000000001</v>
-      </c>
-      <c r="Q25" t="s">
-        <v>230</v>
-      </c>
-      <c r="S25" s="64">
-        <f t="shared" si="0"/>
-        <v>-1.7861933551667386E-3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="s">
         <v>4</v>
       </c>
@@ -3166,30 +2693,8 @@
       <c r="E26" s="56">
         <v>6.4732370000000001</v>
       </c>
-      <c r="L26" t="s">
-        <v>223</v>
-      </c>
-      <c r="M26" s="17">
-        <v>2015</v>
-      </c>
-      <c r="N26" s="12">
-        <v>51.153748</v>
-      </c>
-      <c r="O26" s="12">
-        <v>51.153748</v>
-      </c>
-      <c r="P26" s="12">
-        <v>51.062539999999998</v>
-      </c>
-      <c r="Q26" t="s">
-        <v>230</v>
-      </c>
-      <c r="S26" s="64">
-        <f t="shared" si="0"/>
-        <v>-1.78620178314674E-3</v>
-      </c>
-    </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="11" t="s">
         <v>4</v>
       </c>
@@ -3205,30 +2710,8 @@
       <c r="E27" s="56">
         <v>14.899558000000001</v>
       </c>
-      <c r="L27" t="s">
-        <v>224</v>
-      </c>
-      <c r="M27" s="17">
-        <v>2011</v>
-      </c>
-      <c r="N27" s="12">
-        <v>5.5771870000000003</v>
-      </c>
-      <c r="O27" s="57">
-        <v>5.7327260000000004</v>
-      </c>
-      <c r="P27" s="12">
-        <v>5.5672420000000002</v>
-      </c>
-      <c r="Q27" t="s">
-        <v>228</v>
-      </c>
-      <c r="S27" s="64">
-        <f t="shared" si="0"/>
-        <v>-1.7863423217456852E-3</v>
-      </c>
-    </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="s">
         <v>4</v>
       </c>
@@ -3244,30 +2727,8 @@
       <c r="E28" s="56">
         <v>10.612791</v>
       </c>
-      <c r="L28" t="s">
-        <v>224</v>
-      </c>
-      <c r="M28" s="17">
-        <v>2012</v>
-      </c>
-      <c r="N28" s="12">
-        <v>3.6994479999999998</v>
-      </c>
-      <c r="O28" s="12">
-        <v>3.6994479999999998</v>
-      </c>
-      <c r="P28" s="12">
-        <v>3.6928519999999998</v>
-      </c>
-      <c r="Q28" t="s">
-        <v>228</v>
-      </c>
-      <c r="S28" s="64">
-        <f t="shared" si="0"/>
-        <v>-1.7861533578925034E-3</v>
-      </c>
-    </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="11" t="s">
         <v>4</v>
       </c>
@@ -3283,30 +2744,8 @@
       <c r="E29" s="56">
         <v>9.9698910000000005</v>
       </c>
-      <c r="L29" t="s">
-        <v>224</v>
-      </c>
-      <c r="M29" s="17">
-        <v>2013</v>
-      </c>
-      <c r="N29" s="12">
-        <v>16.269772</v>
-      </c>
-      <c r="O29" s="12">
-        <v>16.269770000000001</v>
-      </c>
-      <c r="P29" s="12">
-        <v>16.240760000000002</v>
-      </c>
-      <c r="Q29" t="s">
-        <v>228</v>
-      </c>
-      <c r="S29" s="64">
-        <f t="shared" si="0"/>
-        <v>-1.7863696033928237E-3</v>
-      </c>
-    </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="s">
         <v>4</v>
       </c>
@@ -3322,30 +2761,8 @@
       <c r="E30" s="56">
         <v>51.153748</v>
       </c>
-      <c r="L30" t="s">
-        <v>224</v>
-      </c>
-      <c r="M30" s="17">
-        <v>2014</v>
-      </c>
-      <c r="N30" s="12">
-        <v>13.206845</v>
-      </c>
-      <c r="O30" s="12">
-        <v>13.206845</v>
-      </c>
-      <c r="P30" s="12">
-        <v>13.183299999999999</v>
-      </c>
-      <c r="Q30" t="s">
-        <v>228</v>
-      </c>
-      <c r="S30" s="64">
-        <f t="shared" si="0"/>
-        <v>-1.7859716459460357E-3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="11" t="s">
         <v>4</v>
       </c>
@@ -3361,30 +2778,8 @@
       <c r="E31" s="56">
         <v>23.588162000000001</v>
       </c>
-      <c r="L31" t="s">
-        <v>224</v>
-      </c>
-      <c r="M31" s="17">
-        <v>2015</v>
-      </c>
-      <c r="N31" s="12">
-        <v>23.588162000000001</v>
-      </c>
-      <c r="O31" s="12">
-        <v>23.588162000000001</v>
-      </c>
-      <c r="P31" s="12">
-        <v>23.546099999999999</v>
-      </c>
-      <c r="Q31" t="s">
-        <v>228</v>
-      </c>
-      <c r="S31" s="64">
-        <f t="shared" si="0"/>
-        <v>-1.7863680184829495E-3</v>
-      </c>
-    </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="11" t="s">
         <v>7</v>
       </c>
@@ -7326,1451 +6721,2167 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R47"/>
+  <dimension ref="A1:AJ47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G56" sqref="G56"/>
+    <sheetView tabSelected="1" zoomScale="101" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="17.42578125" customWidth="1"/>
-    <col min="18" max="18" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="22.85546875" style="15" customWidth="1"/>
+    <col min="5" max="5" width="24.5703125" style="15" customWidth="1"/>
+    <col min="6" max="7" width="9.140625" style="65"/>
+    <col min="8" max="8" width="14.28515625" style="65" bestFit="1" customWidth="1"/>
+    <col min="19" max="25" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="27" max="30" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="17.42578125" customWidth="1"/>
+    <col min="36" max="36" width="19.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B1">
+    <row r="1" spans="1:36" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1" s="63" t="s">
+        <v>218</v>
+      </c>
+      <c r="B1" s="63" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="71" t="s">
+        <v>225</v>
+      </c>
+      <c r="D1" s="73" t="s">
+        <v>226</v>
+      </c>
+      <c r="E1" s="73" t="s">
+        <v>227</v>
+      </c>
+      <c r="F1" s="64"/>
+      <c r="G1" s="64"/>
+      <c r="H1" s="64"/>
+      <c r="T1">
         <v>1</v>
       </c>
-      <c r="C1">
+      <c r="U1">
         <v>2</v>
       </c>
-      <c r="D1">
-        <v>3</v>
-      </c>
-      <c r="E1">
+      <c r="V1">
+        <v>3</v>
+      </c>
+      <c r="W1">
         <v>4</v>
       </c>
-      <c r="F1">
+      <c r="X1">
         <v>5</v>
       </c>
-      <c r="G1">
+      <c r="Y1">
         <v>6</v>
       </c>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="46"/>
-      <c r="L1" s="47"/>
-      <c r="M1" s="48"/>
-      <c r="O1" s="18" t="s">
+      <c r="AA1" s="45"/>
+      <c r="AB1" s="45"/>
+      <c r="AC1" s="46"/>
+      <c r="AD1" s="47"/>
+      <c r="AE1" s="48"/>
+      <c r="AG1" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="P1" t="s">
+      <c r="AH1" t="s">
         <v>53</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="AI1" t="s">
         <v>54</v>
       </c>
-      <c r="R1" t="s">
+      <c r="AJ1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A2" s="66" t="s">
+        <v>219</v>
+      </c>
+      <c r="B2" s="67">
         <v>2011</v>
       </c>
-      <c r="B2">
+      <c r="C2" s="72">
+        <v>23.452044000000001</v>
+      </c>
+      <c r="D2" s="75">
+        <v>29.855460999999998</v>
+      </c>
+      <c r="E2" s="75">
+        <v>9.1240900000000007</v>
+      </c>
+      <c r="F2" s="68" t="s">
+        <v>228</v>
+      </c>
+      <c r="G2" s="68"/>
+      <c r="H2" s="70">
+        <f>(E2-C2)/E2</f>
+        <v>-1.570343343829357</v>
+      </c>
+      <c r="S2">
+        <v>2011</v>
+      </c>
+      <c r="T2">
         <v>23.452043861243041</v>
       </c>
-      <c r="C2">
+      <c r="U2">
         <v>4.5788637788655961</v>
       </c>
-      <c r="D2">
+      <c r="V2">
         <v>1.5885113287342694</v>
       </c>
-      <c r="E2">
+      <c r="W2">
         <v>1.8823994563804169</v>
       </c>
-      <c r="F2">
+      <c r="X2">
         <v>12.486065787224014</v>
       </c>
-      <c r="G2">
+      <c r="Y2">
         <v>0.6482647808533899</v>
       </c>
-      <c r="I2" s="45" t="s">
+      <c r="AA2" s="45" t="s">
         <v>49</v>
       </c>
-      <c r="J2" s="45" t="s">
+      <c r="AB2" s="45" t="s">
         <v>48</v>
       </c>
-      <c r="K2" s="44" t="s">
+      <c r="AC2" s="44" t="s">
         <v>51</v>
       </c>
-      <c r="L2" s="44" t="s">
+      <c r="AD2" s="44" t="s">
         <v>50</v>
       </c>
-      <c r="M2" s="44" t="s">
+      <c r="AE2" s="44" t="s">
         <v>52</v>
       </c>
-      <c r="O2" s="19">
+      <c r="AG2" s="19">
         <v>1</v>
       </c>
-      <c r="P2" s="17">
+      <c r="AH2" s="17">
         <v>83.67654603862178</v>
       </c>
-      <c r="Q2" s="17">
+      <c r="AI2" s="17">
         <v>72.507093987073105</v>
       </c>
-      <c r="R2" s="17">
+      <c r="AJ2" s="17">
         <v>11.581627299951531</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A3" s="66" t="s">
+        <v>219</v>
+      </c>
+      <c r="B3" s="67">
         <v>2012</v>
       </c>
-      <c r="B3">
+      <c r="C3" s="72">
+        <v>11.148345000000001</v>
+      </c>
+      <c r="D3" s="74">
+        <v>11.148345000000001</v>
+      </c>
+      <c r="E3" s="75">
+        <v>14.43534</v>
+      </c>
+      <c r="F3" s="68" t="s">
+        <v>228</v>
+      </c>
+      <c r="G3" s="68"/>
+      <c r="H3" s="70">
+        <f>(E3-C3)/E3</f>
+        <v>0.22770471634197734</v>
+      </c>
+      <c r="S3">
+        <v>2012</v>
+      </c>
+      <c r="T3">
         <v>11.148345111979213</v>
       </c>
-      <c r="C3">
+      <c r="U3">
         <v>12.322574278492283</v>
       </c>
-      <c r="D3">
+      <c r="V3">
         <v>4.2925414474434866</v>
       </c>
-      <c r="E3">
+      <c r="W3">
         <v>5.9977010626825571</v>
       </c>
-      <c r="F3">
+      <c r="X3">
         <v>7.7289411623128679</v>
       </c>
-      <c r="G3">
+      <c r="Y3">
         <v>3.6994482564836635</v>
       </c>
-      <c r="I3" s="1">
+      <c r="AA3" s="1">
         <v>1</v>
       </c>
-      <c r="J3" s="1">
+      <c r="AB3" s="1">
         <v>2011</v>
       </c>
-      <c r="K3" s="39">
+      <c r="AC3" s="39">
         <v>3.7678100933982313</v>
       </c>
-      <c r="L3" s="40">
+      <c r="AD3" s="40">
         <v>23.452043861243041</v>
       </c>
-      <c r="M3" s="41">
-        <f t="shared" ref="M3:M32" si="0">L3-K3</f>
+      <c r="AE3" s="41">
+        <f t="shared" ref="AE3:AE32" si="0">AD3-AC3</f>
         <v>19.684233767844809</v>
       </c>
-      <c r="O3" s="19">
+      <c r="AG3" s="19">
         <v>2</v>
       </c>
-      <c r="P3" s="17">
+      <c r="AH3" s="17">
         <v>123.17066418316776</v>
       </c>
-      <c r="Q3" s="17">
+      <c r="AI3" s="17">
         <v>143.74592102263361</v>
       </c>
-      <c r="R3" s="17">
+      <c r="AJ3" s="17">
         <v>14.295345860773452</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A4" s="66" t="s">
+        <v>219</v>
+      </c>
+      <c r="B4" s="67">
         <v>2013</v>
       </c>
-      <c r="B4">
+      <c r="C4" s="72">
+        <v>20.605733000000001</v>
+      </c>
+      <c r="D4" s="74">
+        <v>20.605730000000001</v>
+      </c>
+      <c r="E4" s="75">
+        <v>23.84834</v>
+      </c>
+      <c r="F4" s="68" t="s">
+        <v>228</v>
+      </c>
+      <c r="G4" s="68"/>
+      <c r="H4" s="70">
+        <f>(E4-C4)/E4</f>
+        <v>0.13596782836876695</v>
+      </c>
+      <c r="S4">
+        <v>2013</v>
+      </c>
+      <c r="T4">
         <v>20.605732597297074</v>
       </c>
-      <c r="C4">
+      <c r="U4">
         <v>32.226103252712221</v>
       </c>
-      <c r="D4">
+      <c r="V4">
         <v>19.10728323177532</v>
       </c>
-      <c r="E4">
+      <c r="W4">
         <v>20.814663293615897</v>
       </c>
-      <c r="F4">
+      <c r="X4">
         <v>36.214896617535196</v>
       </c>
-      <c r="G4">
+      <c r="Y4">
         <v>16.269771518398983</v>
       </c>
-      <c r="I4" s="1">
+      <c r="AA4" s="1">
         <v>1</v>
       </c>
-      <c r="J4" s="1">
+      <c r="AB4" s="1">
         <v>2012</v>
       </c>
-      <c r="K4" s="39">
+      <c r="AC4" s="39">
         <v>14.430646157550678</v>
       </c>
-      <c r="L4" s="40">
+      <c r="AD4" s="40">
         <v>11.148345111979213</v>
       </c>
-      <c r="M4" s="41">
+      <c r="AE4" s="41">
         <f t="shared" si="0"/>
         <v>-3.2823010455714652</v>
       </c>
-      <c r="O4" s="19">
-        <v>3</v>
-      </c>
-      <c r="P4" s="17">
+      <c r="AG4" s="19">
+        <v>3</v>
+      </c>
+      <c r="AH4" s="17">
         <v>42.043699336551775</v>
       </c>
-      <c r="Q4" s="17">
+      <c r="AI4" s="17">
         <v>49.639974327155869</v>
       </c>
-      <c r="R4" s="17">
+      <c r="AJ4" s="17">
         <v>6.7616306969909976</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A5">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A5" s="66" t="s">
+        <v>219</v>
+      </c>
+      <c r="B5" s="67">
         <v>2014</v>
       </c>
-      <c r="B5">
+      <c r="C5" s="72">
+        <v>21.997187</v>
+      </c>
+      <c r="D5" s="74">
+        <v>21.997187</v>
+      </c>
+      <c r="E5" s="75">
+        <v>37.060639999999999</v>
+      </c>
+      <c r="F5" s="68" t="s">
+        <v>228</v>
+      </c>
+      <c r="G5" s="68"/>
+      <c r="H5" s="70">
+        <f>(E5-C5)/E5</f>
+        <v>0.40645420586368719</v>
+      </c>
+      <c r="S5">
+        <v>2014</v>
+      </c>
+      <c r="T5">
         <v>21.997187461853823</v>
       </c>
-      <c r="C5">
+      <c r="U5">
         <v>59.143658115801664</v>
       </c>
-      <c r="D5">
+      <c r="V5">
         <v>6.4460640319366291</v>
       </c>
-      <c r="E5">
+      <c r="W5">
         <v>15.617248728120618</v>
       </c>
-      <c r="F5">
+      <c r="X5">
         <v>55.974492961519047</v>
       </c>
-      <c r="G5">
+      <c r="Y5">
         <v>13.206844518128886</v>
       </c>
-      <c r="I5" s="1">
+      <c r="AA5" s="1">
         <v>1</v>
       </c>
-      <c r="J5" s="1">
+      <c r="AB5" s="1">
         <v>2013</v>
       </c>
-      <c r="K5" s="39">
+      <c r="AC5" s="39">
         <v>24.026385480314023</v>
       </c>
-      <c r="L5" s="40">
+      <c r="AD5" s="40">
         <v>20.605732597297074</v>
       </c>
-      <c r="M5" s="41">
+      <c r="AE5" s="41">
         <f t="shared" si="0"/>
         <v>-3.4206528830169489</v>
       </c>
-      <c r="O5" s="19">
+      <c r="AG5" s="19">
         <v>4</v>
       </c>
-      <c r="P5" s="17">
+      <c r="AH5" s="17">
         <v>109.30771614249772</v>
       </c>
-      <c r="Q5" s="17">
+      <c r="AI5" s="17">
         <v>51.240479278924411</v>
       </c>
-      <c r="R5" s="17">
+      <c r="AJ5" s="17">
         <v>6.2715178235496234</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A6">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A6" s="66" t="s">
+        <v>219</v>
+      </c>
+      <c r="B6" s="67">
         <v>2015</v>
       </c>
-      <c r="B6">
+      <c r="C6" s="72">
+        <v>6.4732370000000001</v>
+      </c>
+      <c r="D6" s="74">
+        <v>6.4732370000000001</v>
+      </c>
+      <c r="E6" s="75">
+        <v>10.604950000000001</v>
+      </c>
+      <c r="F6" s="68" t="s">
+        <v>228</v>
+      </c>
+      <c r="G6" s="68"/>
+      <c r="H6" s="70">
+        <f>(E6-C6)/E6</f>
+        <v>0.38960230835600357</v>
+      </c>
+      <c r="S6">
+        <v>2015</v>
+      </c>
+      <c r="T6">
         <v>6.4732370062486293</v>
       </c>
-      <c r="C6">
+      <c r="U6">
         <v>14.899464757295986</v>
       </c>
-      <c r="D6">
+      <c r="V6">
         <v>10.609299296662067</v>
       </c>
-      <c r="E6">
+      <c r="W6">
         <v>64.995703601698239</v>
       </c>
-      <c r="F6">
+      <c r="X6">
         <v>51.15374766070407</v>
       </c>
-      <c r="G6">
+      <c r="Y6">
         <v>23.588162023184807</v>
       </c>
-      <c r="I6" s="1">
+      <c r="AA6" s="1">
         <v>1</v>
       </c>
-      <c r="J6" s="1">
+      <c r="AB6" s="1">
         <v>2014</v>
       </c>
-      <c r="K6" s="39">
+      <c r="AC6" s="39">
         <v>30.282252255810182</v>
       </c>
-      <c r="L6" s="40">
+      <c r="AD6" s="40">
         <v>21.997187461853823</v>
       </c>
-      <c r="M6" s="41">
+      <c r="AE6" s="41">
         <f t="shared" si="0"/>
         <v>-8.2850647939563586</v>
       </c>
-      <c r="O6" s="19">
+      <c r="AG6" s="19">
         <v>5</v>
       </c>
-      <c r="P6" s="17">
+      <c r="AH6" s="17">
         <v>163.55814418929521</v>
       </c>
-      <c r="Q6" s="17">
+      <c r="AI6" s="17">
         <v>118.01627490523558</v>
       </c>
-      <c r="R6" s="17">
+      <c r="AJ6" s="17">
         <v>20.9251900340021</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="I7" s="42">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A7" s="66" t="s">
+        <v>220</v>
+      </c>
+      <c r="B7" s="67">
+        <v>2011</v>
+      </c>
+      <c r="C7" s="72">
+        <v>30.218699000000001</v>
+      </c>
+      <c r="D7" s="75">
+        <v>42.465522999999997</v>
+      </c>
+      <c r="E7" s="74">
+        <v>30.164850000000001</v>
+      </c>
+      <c r="F7" s="68" t="s">
+        <v>230</v>
+      </c>
+      <c r="G7" s="68"/>
+      <c r="H7" s="69">
+        <f>(E7-C7)/E7</f>
+        <v>-1.7851572277004391E-3</v>
+      </c>
+      <c r="AA7" s="42">
         <v>1</v>
       </c>
-      <c r="J7" s="42">
+      <c r="AB7" s="42">
         <v>2015</v>
       </c>
-      <c r="K7" s="43"/>
-      <c r="L7" s="40">
+      <c r="AC7" s="43"/>
+      <c r="AD7" s="40">
         <v>6.4732370062486293</v>
       </c>
-      <c r="M7" s="41">
+      <c r="AE7" s="41">
         <f t="shared" si="0"/>
         <v>6.4732370062486293</v>
       </c>
-      <c r="O7" s="19">
+      <c r="AG7" s="19">
         <v>6</v>
       </c>
-      <c r="P7" s="17">
+      <c r="AH7" s="17">
         <v>57.412491097049724</v>
       </c>
-      <c r="Q7" s="17">
+      <c r="AI7" s="17">
         <v>36.940560256917017</v>
       </c>
-      <c r="R7" s="17">
+      <c r="AJ7" s="17">
         <v>5.6451720657715097</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B8">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A8" s="66" t="s">
+        <v>220</v>
+      </c>
+      <c r="B8" s="67">
+        <v>2012</v>
+      </c>
+      <c r="C8" s="72">
+        <v>12.322573999999999</v>
+      </c>
+      <c r="D8" s="74">
+        <v>12.322573999999999</v>
+      </c>
+      <c r="E8" s="74">
+        <v>12.300599999999999</v>
+      </c>
+      <c r="F8" s="68" t="s">
+        <v>230</v>
+      </c>
+      <c r="G8" s="68"/>
+      <c r="H8" s="69">
+        <f>(E8-C8)/E8</f>
+        <v>-1.7864169227517488E-3</v>
+      </c>
+      <c r="T8">
         <v>2011</v>
       </c>
-      <c r="C8">
+      <c r="U8">
         <v>2012</v>
       </c>
-      <c r="D8">
+      <c r="V8">
         <v>2013</v>
       </c>
-      <c r="E8">
+      <c r="W8">
         <v>2014</v>
       </c>
-      <c r="F8">
+      <c r="X8">
         <v>2015</v>
       </c>
-      <c r="I8" s="1">
+      <c r="AA8" s="1">
         <v>2</v>
       </c>
-      <c r="J8" s="1">
+      <c r="AB8" s="1">
         <v>2011</v>
       </c>
-      <c r="K8" s="39">
+      <c r="AC8" s="39">
         <v>30.246969564684228</v>
       </c>
-      <c r="L8" s="40">
+      <c r="AD8" s="40">
         <v>4.5788637788655961</v>
       </c>
-      <c r="M8" s="41">
+      <c r="AE8" s="41">
         <f t="shared" si="0"/>
         <v>-25.668105785818632</v>
       </c>
-      <c r="O8" s="19" t="s">
+      <c r="AG8" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="P8" s="17">
+      <c r="AH8" s="17">
         <v>579.16926098718409</v>
       </c>
-      <c r="Q8" s="17">
+      <c r="AI8" s="17">
         <v>472.0903037779396</v>
       </c>
-      <c r="R8" s="17">
+      <c r="AJ8" s="17">
         <v>14.698691968952467</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A9">
+    <row r="9" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A9" s="66" t="s">
+        <v>220</v>
+      </c>
+      <c r="B9" s="67">
+        <v>2013</v>
+      </c>
+      <c r="C9" s="72">
+        <v>32.226103000000002</v>
+      </c>
+      <c r="D9" s="74">
+        <v>32.226100000000002</v>
+      </c>
+      <c r="E9" s="74">
+        <v>32.168640000000003</v>
+      </c>
+      <c r="F9" s="68" t="s">
+        <v>230</v>
+      </c>
+      <c r="G9" s="68"/>
+      <c r="H9" s="69">
+        <f>(E9-C9)/E9</f>
+        <v>-1.7863049230554503E-3</v>
+      </c>
+      <c r="S9">
         <v>1</v>
       </c>
-      <c r="B9">
+      <c r="T9">
         <v>23.452043861243041</v>
       </c>
-      <c r="C9">
+      <c r="U9">
         <v>11.148345111979213</v>
       </c>
-      <c r="D9">
+      <c r="V9">
         <v>20.605732597297074</v>
       </c>
-      <c r="E9">
+      <c r="W9">
         <v>21.997187461853823</v>
       </c>
-      <c r="F9">
+      <c r="X9">
         <v>6.4732370062486293</v>
       </c>
-      <c r="I9" s="1">
+      <c r="AA9" s="1">
         <v>2</v>
       </c>
-      <c r="J9" s="1">
+      <c r="AB9" s="1">
         <v>2012</v>
       </c>
-      <c r="K9" s="39">
+      <c r="AC9" s="39">
         <v>24.597632137224569</v>
       </c>
-      <c r="L9" s="40">
+      <c r="AD9" s="40">
         <v>12.322574278492283</v>
       </c>
-      <c r="M9" s="41">
+      <c r="AE9" s="41">
         <f t="shared" si="0"/>
         <v>-12.275057858732286</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A10">
+    <row r="10" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A10" s="66" t="s">
+        <v>220</v>
+      </c>
+      <c r="B10" s="67">
+        <v>2014</v>
+      </c>
+      <c r="C10" s="72">
+        <v>59.143658000000002</v>
+      </c>
+      <c r="D10" s="74">
+        <v>59.143658000000002</v>
+      </c>
+      <c r="E10" s="74">
+        <v>59.038209999999999</v>
+      </c>
+      <c r="F10" s="68" t="s">
+        <v>230</v>
+      </c>
+      <c r="G10" s="68"/>
+      <c r="H10" s="69">
+        <f>(E10-C10)/E10</f>
+        <v>-1.7860975121028E-3</v>
+      </c>
+      <c r="S10">
         <v>2</v>
       </c>
-      <c r="B10">
+      <c r="T10">
         <v>4.5788637788655961</v>
       </c>
-      <c r="C10">
+      <c r="U10">
         <v>12.322574278492283</v>
       </c>
-      <c r="D10">
+      <c r="V10">
         <v>32.226103252712221</v>
       </c>
-      <c r="E10">
+      <c r="W10">
         <v>59.143658115801664</v>
       </c>
-      <c r="F10">
+      <c r="X10">
         <v>14.899464757295986</v>
       </c>
-      <c r="I10" s="1">
+      <c r="AA10" s="1">
         <v>2</v>
       </c>
-      <c r="J10" s="1">
+      <c r="AB10" s="1">
         <v>2013</v>
       </c>
-      <c r="K10" s="39">
+      <c r="AC10" s="39">
         <v>32.058157301863403</v>
       </c>
-      <c r="L10" s="40">
+      <c r="AD10" s="40">
         <v>32.226103252712221</v>
       </c>
-      <c r="M10" s="41">
+      <c r="AE10" s="41">
         <f t="shared" si="0"/>
         <v>0.16794595084881792</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>3</v>
-      </c>
-      <c r="B11">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A11" s="66" t="s">
+        <v>220</v>
+      </c>
+      <c r="B11" s="67">
+        <v>2015</v>
+      </c>
+      <c r="C11" s="72">
+        <v>14.899464999999999</v>
+      </c>
+      <c r="D11" s="74">
+        <v>14.899558000000001</v>
+      </c>
+      <c r="E11" s="74">
+        <v>14.8729</v>
+      </c>
+      <c r="F11" s="68" t="s">
+        <v>230</v>
+      </c>
+      <c r="G11" s="68"/>
+      <c r="H11" s="69">
+        <f>(E11-C11)/E11</f>
+        <v>-1.7861345131077145E-3</v>
+      </c>
+      <c r="S11">
+        <v>3</v>
+      </c>
+      <c r="T11">
         <v>1.5885113287342694</v>
       </c>
-      <c r="C11">
+      <c r="U11">
         <v>4.2925414474434866</v>
       </c>
-      <c r="D11">
+      <c r="V11">
         <v>19.10728323177532</v>
       </c>
-      <c r="E11">
+      <c r="W11">
         <v>6.4460640319366291</v>
       </c>
-      <c r="F11">
+      <c r="X11">
         <v>10.609299296662067</v>
       </c>
-      <c r="I11" s="1">
+      <c r="AA11" s="1">
         <v>2</v>
       </c>
-      <c r="J11" s="1">
+      <c r="AB11" s="1">
         <v>2014</v>
       </c>
-      <c r="K11" s="39">
+      <c r="AC11" s="39">
         <v>56.843162018861399</v>
       </c>
-      <c r="L11" s="40">
+      <c r="AD11" s="40">
         <v>59.143658115801664</v>
       </c>
-      <c r="M11" s="41">
+      <c r="AE11" s="41">
         <f t="shared" si="0"/>
         <v>2.3004960969402646</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A12">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A12" s="66" t="s">
+        <v>221</v>
+      </c>
+      <c r="B12" s="67">
+        <v>2011</v>
+      </c>
+      <c r="C12" s="72">
+        <v>9.6991209999999999</v>
+      </c>
+      <c r="D12" s="75">
+        <v>11.357567</v>
+      </c>
+      <c r="E12" s="74">
+        <v>9.6818270000000002</v>
+      </c>
+      <c r="F12" s="68" t="s">
+        <v>229</v>
+      </c>
+      <c r="G12" s="68"/>
+      <c r="H12" s="69">
+        <f>(E12-C12)/E12</f>
+        <v>-1.7862331148862398E-3</v>
+      </c>
+      <c r="S12">
         <v>4</v>
       </c>
-      <c r="B12">
+      <c r="T12">
         <v>1.8823994563804169</v>
       </c>
-      <c r="C12">
+      <c r="U12">
         <v>5.9977010626825571</v>
       </c>
-      <c r="D12">
+      <c r="V12">
         <v>20.814663293615897</v>
       </c>
-      <c r="E12">
+      <c r="W12">
         <v>15.617248728120618</v>
       </c>
-      <c r="F12">
+      <c r="X12">
         <v>64.995703601698239</v>
       </c>
-      <c r="I12" s="1">
+      <c r="AA12" s="1">
         <v>2</v>
       </c>
-      <c r="J12" s="42">
+      <c r="AB12" s="42">
         <v>2015</v>
       </c>
-      <c r="K12" s="43"/>
-      <c r="L12" s="40">
+      <c r="AC12" s="43"/>
+      <c r="AD12" s="40">
         <v>14.899464757295986</v>
       </c>
-      <c r="M12" s="41">
+      <c r="AE12" s="41">
         <f t="shared" si="0"/>
         <v>14.899464757295986</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A13">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A13" s="66" t="s">
+        <v>221</v>
+      </c>
+      <c r="B13" s="67">
+        <v>2012</v>
+      </c>
+      <c r="C13" s="72">
+        <v>4.2925409999999999</v>
+      </c>
+      <c r="D13" s="74">
+        <v>4.2925409999999999</v>
+      </c>
+      <c r="E13" s="74">
+        <v>4.2848879999999996</v>
+      </c>
+      <c r="F13" s="68" t="s">
+        <v>229</v>
+      </c>
+      <c r="G13" s="68"/>
+      <c r="H13" s="69">
+        <f>(E13-C13)/E13</f>
+        <v>-1.7860443493506375E-3</v>
+      </c>
+      <c r="S13">
         <v>5</v>
       </c>
-      <c r="B13">
+      <c r="T13">
         <v>12.486065787224014</v>
       </c>
-      <c r="C13">
+      <c r="U13">
         <v>7.7289411623128679</v>
       </c>
-      <c r="D13">
+      <c r="V13">
         <v>36.214896617535196</v>
       </c>
-      <c r="E13">
+      <c r="W13">
         <v>55.974492961519047</v>
       </c>
-      <c r="F13">
+      <c r="X13">
         <v>51.15374766070407</v>
       </c>
-      <c r="I13" s="1">
-        <v>3</v>
-      </c>
-      <c r="J13" s="1">
+      <c r="AA13" s="1">
+        <v>3</v>
+      </c>
+      <c r="AB13" s="1">
         <v>2011</v>
       </c>
-      <c r="K13" s="39">
+      <c r="AC13" s="39">
         <v>9.7031163052810268</v>
       </c>
-      <c r="L13" s="40">
+      <c r="AD13" s="40">
         <v>1.5885113287342694</v>
       </c>
-      <c r="M13" s="41">
+      <c r="AE13" s="41">
         <f t="shared" si="0"/>
         <v>-8.1146049765467581</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A14">
+    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A14" s="66" t="s">
+        <v>221</v>
+      </c>
+      <c r="B14" s="67">
+        <v>2013</v>
+      </c>
+      <c r="C14" s="72">
+        <v>19.107282999999999</v>
+      </c>
+      <c r="D14" s="74">
+        <v>19.107279999999999</v>
+      </c>
+      <c r="E14" s="74">
+        <v>19.07321</v>
+      </c>
+      <c r="F14" s="68" t="s">
+        <v>229</v>
+      </c>
+      <c r="G14" s="68"/>
+      <c r="H14" s="69">
+        <f>(E14-C14)/E14</f>
+        <v>-1.7864323834320156E-3</v>
+      </c>
+      <c r="S14">
         <v>6</v>
       </c>
-      <c r="B14">
+      <c r="T14">
         <v>0.6482647808533899</v>
       </c>
-      <c r="C14">
+      <c r="U14">
         <v>3.6994482564836635</v>
       </c>
-      <c r="D14">
+      <c r="V14">
         <v>16.269771518398983</v>
       </c>
-      <c r="E14">
+      <c r="W14">
         <v>13.206844518128886</v>
       </c>
-      <c r="F14">
+      <c r="X14">
         <v>23.588162023184807</v>
       </c>
-      <c r="I14" s="1">
-        <v>3</v>
-      </c>
-      <c r="J14" s="1">
+      <c r="AA14" s="1">
+        <v>3</v>
+      </c>
+      <c r="AB14" s="1">
         <v>2012</v>
       </c>
-      <c r="K14" s="39">
+      <c r="AC14" s="39">
         <v>4.2278309234767981</v>
       </c>
-      <c r="L14" s="40">
+      <c r="AD14" s="40">
         <v>4.2925414474434866</v>
       </c>
-      <c r="M14" s="41">
+      <c r="AE14" s="41">
         <f t="shared" si="0"/>
         <v>6.4710523966688527E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="I15" s="1">
-        <v>3</v>
-      </c>
-      <c r="J15" s="1">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A15" s="66" t="s">
+        <v>221</v>
+      </c>
+      <c r="B15" s="67">
+        <v>2014</v>
+      </c>
+      <c r="C15" s="72">
+        <v>6.4460639999999998</v>
+      </c>
+      <c r="D15" s="74">
+        <v>6.4460639999999998</v>
+      </c>
+      <c r="E15" s="74">
+        <v>6.434571</v>
+      </c>
+      <c r="F15" s="68" t="s">
+        <v>229</v>
+      </c>
+      <c r="G15" s="68"/>
+      <c r="H15" s="69">
+        <f>(E15-C15)/E15</f>
+        <v>-1.7861330615513845E-3</v>
+      </c>
+      <c r="AA15" s="1">
+        <v>3</v>
+      </c>
+      <c r="AB15" s="1">
         <v>2013</v>
       </c>
-      <c r="K15" s="39">
+      <c r="AC15" s="39">
         <v>19.195853054929469</v>
       </c>
-      <c r="L15" s="40">
+      <c r="AD15" s="40">
         <v>19.10728323177532</v>
       </c>
-      <c r="M15" s="41">
+      <c r="AE15" s="41">
         <f t="shared" si="0"/>
         <v>-8.8569823154148963E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A16" s="61" t="s">
+    <row r="16" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A16" s="66" t="s">
+        <v>221</v>
+      </c>
+      <c r="B16" s="67">
+        <v>2015</v>
+      </c>
+      <c r="C16" s="72">
+        <v>10.609299</v>
+      </c>
+      <c r="D16" s="74">
+        <v>10.612791</v>
+      </c>
+      <c r="E16" s="74">
+        <v>10.59038</v>
+      </c>
+      <c r="F16" s="68" t="s">
+        <v>229</v>
+      </c>
+      <c r="G16" s="68"/>
+      <c r="H16" s="69">
+        <f>(E16-C16)/E16</f>
+        <v>-1.7864325925982215E-3</v>
+      </c>
+      <c r="S16" s="61" t="s">
         <v>49</v>
       </c>
-      <c r="B16" s="61" t="s">
+      <c r="T16" s="61" t="s">
         <v>48</v>
       </c>
-      <c r="C16" s="58" t="s">
+      <c r="U16" s="58" t="s">
         <v>47</v>
       </c>
-      <c r="D16" s="59"/>
-      <c r="E16" s="60"/>
-      <c r="I16" s="1">
-        <v>3</v>
-      </c>
-      <c r="J16" s="1">
+      <c r="V16" s="59"/>
+      <c r="W16" s="60"/>
+      <c r="AA16" s="1">
+        <v>3</v>
+      </c>
+      <c r="AB16" s="1">
         <v>2014</v>
       </c>
-      <c r="K16" s="39">
+      <c r="AC16" s="39">
         <v>16.51317404346857</v>
       </c>
-      <c r="L16" s="40">
+      <c r="AD16" s="40">
         <v>6.4460640319366291</v>
       </c>
-      <c r="M16" s="41">
+      <c r="AE16" s="41">
         <f t="shared" si="0"/>
         <v>-10.067110011531941</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="62"/>
-      <c r="B17" s="62"/>
-      <c r="C17" s="44" t="s">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A17" s="66" t="s">
+        <v>222</v>
+      </c>
+      <c r="B17" s="67">
+        <v>2011</v>
+      </c>
+      <c r="C17" s="72">
+        <v>9.5850329999999992</v>
+      </c>
+      <c r="D17" s="75">
+        <v>10.164596</v>
+      </c>
+      <c r="E17" s="74">
+        <v>9.5679420000000004</v>
+      </c>
+      <c r="F17" s="68" t="s">
+        <v>229</v>
+      </c>
+      <c r="G17" s="68"/>
+      <c r="H17" s="69">
+        <f>(E17-C17)/E17</f>
+        <v>-1.7862775505954004E-3</v>
+      </c>
+      <c r="S17" s="62"/>
+      <c r="T17" s="62"/>
+      <c r="U17" s="44" t="s">
         <v>51</v>
       </c>
-      <c r="D17" s="44" t="s">
+      <c r="V17" s="44" t="s">
         <v>50</v>
       </c>
-      <c r="E17" s="44" t="s">
+      <c r="W17" s="44" t="s">
         <v>52</v>
       </c>
-      <c r="I17" s="1">
-        <v>3</v>
-      </c>
-      <c r="J17" s="42">
+      <c r="AA17" s="1">
+        <v>3</v>
+      </c>
+      <c r="AB17" s="42">
         <v>2015</v>
       </c>
-      <c r="K17" s="43"/>
-      <c r="L17" s="40">
+      <c r="AC17" s="43"/>
+      <c r="AD17" s="40">
         <v>10.609299296662067</v>
       </c>
-      <c r="M17" s="41">
+      <c r="AE17" s="41">
         <f t="shared" si="0"/>
         <v>10.609299296662067</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
+    <row r="18" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A18" s="66" t="s">
+        <v>222</v>
+      </c>
+      <c r="B18" s="67">
+        <v>2012</v>
+      </c>
+      <c r="C18" s="72">
+        <v>5.9977010000000002</v>
+      </c>
+      <c r="D18" s="74">
+        <v>5.9977010000000002</v>
+      </c>
+      <c r="E18" s="74">
+        <v>5.9870070000000002</v>
+      </c>
+      <c r="F18" s="68" t="s">
+        <v>229</v>
+      </c>
+      <c r="G18" s="68"/>
+      <c r="H18" s="69">
+        <f>(E18-C18)/E18</f>
+        <v>-1.7862013523618698E-3</v>
+      </c>
+      <c r="S18" s="1">
         <v>1</v>
       </c>
-      <c r="B18" s="1">
+      <c r="T18" s="1">
         <v>2011</v>
       </c>
-      <c r="C18" s="39">
+      <c r="U18" s="39">
         <v>3.7678100933982313</v>
       </c>
-      <c r="D18" s="54">
+      <c r="V18" s="54">
         <v>23.452043861243041</v>
       </c>
-      <c r="E18" s="41">
-        <f>D18-C18</f>
+      <c r="W18" s="41">
+        <f>V18-U18</f>
         <v>19.684233767844809</v>
       </c>
-      <c r="I18" s="1">
+      <c r="AA18" s="1">
         <v>4</v>
       </c>
-      <c r="J18" s="1">
+      <c r="AB18" s="1">
         <v>2011</v>
       </c>
-      <c r="K18" s="39">
+      <c r="AC18" s="39">
         <v>9.5670089828788978</v>
       </c>
-      <c r="L18" s="40">
+      <c r="AD18" s="40">
         <v>1.8823994563804169</v>
       </c>
-      <c r="M18" s="41">
+      <c r="AE18" s="41">
         <f t="shared" si="0"/>
         <v>-7.6846095264984804</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
+    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A19" s="66" t="s">
+        <v>222</v>
+      </c>
+      <c r="B19" s="67">
+        <v>2013</v>
+      </c>
+      <c r="C19" s="72">
+        <v>20.814662999999999</v>
+      </c>
+      <c r="D19" s="74">
+        <v>20.81466</v>
+      </c>
+      <c r="E19" s="74">
+        <v>20.777550000000002</v>
+      </c>
+      <c r="F19" s="68" t="s">
+        <v>229</v>
+      </c>
+      <c r="G19" s="68"/>
+      <c r="H19" s="69">
+        <f>(E19-C19)/E19</f>
+        <v>-1.7862067471861674E-3</v>
+      </c>
+      <c r="S19" s="1">
         <v>2</v>
       </c>
-      <c r="B19" s="1">
+      <c r="T19" s="1">
         <v>2011</v>
       </c>
-      <c r="C19" s="53">
+      <c r="U19" s="53">
         <v>30.246969564684228</v>
       </c>
-      <c r="D19" s="52">
+      <c r="V19" s="52">
         <v>4.5788637788655961</v>
       </c>
-      <c r="E19" s="41">
-        <f t="shared" ref="E19:E47" si="1">D19-C19</f>
+      <c r="W19" s="41">
+        <f t="shared" ref="W19:W47" si="1">V19-U19</f>
         <v>-25.668105785818632</v>
       </c>
-      <c r="I19" s="1">
+      <c r="AA19" s="1">
         <v>4</v>
       </c>
-      <c r="J19" s="1">
+      <c r="AB19" s="1">
         <v>2012</v>
       </c>
-      <c r="K19" s="39">
+      <c r="AC19" s="39">
         <v>5.9905108913495493</v>
       </c>
-      <c r="L19" s="40">
+      <c r="AD19" s="40">
         <v>5.9977010626825571</v>
       </c>
-      <c r="M19" s="41">
+      <c r="AE19" s="41">
         <f t="shared" si="0"/>
         <v>7.190171333007811E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
-        <v>3</v>
-      </c>
-      <c r="B20" s="1">
+    <row r="20" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A20" s="66" t="s">
+        <v>222</v>
+      </c>
+      <c r="B20" s="67">
+        <v>2014</v>
+      </c>
+      <c r="C20" s="72">
+        <v>15.617248999999999</v>
+      </c>
+      <c r="D20" s="74">
+        <v>15.617248999999999</v>
+      </c>
+      <c r="E20" s="74">
+        <v>15.589399999999999</v>
+      </c>
+      <c r="F20" s="68" t="s">
+        <v>229</v>
+      </c>
+      <c r="G20" s="68"/>
+      <c r="H20" s="69">
+        <f>(E20-C20)/E20</f>
+        <v>-1.7864061477670592E-3</v>
+      </c>
+      <c r="S20" s="1">
+        <v>3</v>
+      </c>
+      <c r="T20" s="1">
         <v>2011</v>
       </c>
-      <c r="C20" s="53">
+      <c r="U20" s="53">
         <v>9.7031163052810268</v>
       </c>
-      <c r="D20" s="52">
+      <c r="V20" s="52">
         <v>1.5885113287342694</v>
       </c>
-      <c r="E20" s="41">
+      <c r="W20" s="41">
         <f t="shared" si="1"/>
         <v>-8.1146049765467581</v>
       </c>
-      <c r="G20" t="s">
+      <c r="Y20" t="s">
         <v>56</v>
       </c>
-      <c r="I20" s="1">
+      <c r="AA20" s="1">
         <v>4</v>
       </c>
-      <c r="J20" s="1">
+      <c r="AB20" s="1">
         <v>2013</v>
       </c>
-      <c r="K20" s="39">
+      <c r="AC20" s="39">
         <v>20.115441999783801</v>
       </c>
-      <c r="L20" s="40">
+      <c r="AD20" s="40">
         <v>20.814663293615897</v>
       </c>
-      <c r="M20" s="41">
+      <c r="AE20" s="41">
         <f t="shared" si="0"/>
         <v>0.69922129383209608</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
+    <row r="21" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A21" s="66" t="s">
+        <v>222</v>
+      </c>
+      <c r="B21" s="67">
+        <v>2015</v>
+      </c>
+      <c r="C21" s="72">
+        <v>9.9696359999999995</v>
+      </c>
+      <c r="D21" s="74">
+        <v>9.9698910000000005</v>
+      </c>
+      <c r="E21" s="74">
+        <v>9.9518599999999999</v>
+      </c>
+      <c r="F21" s="68" t="s">
+        <v>229</v>
+      </c>
+      <c r="G21" s="68"/>
+      <c r="H21" s="69">
+        <f>(E21-C21)/E21</f>
+        <v>-1.7861987608346148E-3</v>
+      </c>
+      <c r="S21" s="1">
         <v>4</v>
       </c>
-      <c r="B21" s="1">
+      <c r="T21" s="1">
         <v>2011</v>
       </c>
-      <c r="C21" s="53">
+      <c r="U21" s="53">
         <v>9.5670089828788978</v>
       </c>
-      <c r="D21" s="52">
+      <c r="V21" s="52">
         <v>1.8823994563804169</v>
       </c>
-      <c r="E21" s="41">
+      <c r="W21" s="41">
         <f t="shared" si="1"/>
         <v>-7.6846095264984804</v>
       </c>
-      <c r="I21" s="1">
+      <c r="AA21" s="1">
         <v>4</v>
       </c>
-      <c r="J21" s="1">
+      <c r="AB21" s="1">
         <v>2014</v>
       </c>
-      <c r="K21" s="39">
+      <c r="AC21" s="39">
         <v>15.567517404912163</v>
       </c>
-      <c r="L21" s="40">
+      <c r="AD21" s="40">
         <v>15.617248728120618</v>
       </c>
-      <c r="M21" s="41">
+      <c r="AE21" s="41">
         <f t="shared" si="0"/>
         <v>4.973132320845508E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
+    <row r="22" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A22" s="66" t="s">
+        <v>223</v>
+      </c>
+      <c r="B22" s="67">
+        <v>2011</v>
+      </c>
+      <c r="C22" s="72">
+        <v>19.045133</v>
+      </c>
+      <c r="D22" s="75">
+        <v>24.493995999999999</v>
+      </c>
+      <c r="E22" s="74">
+        <v>19.01118</v>
+      </c>
+      <c r="F22" s="68" t="s">
+        <v>230</v>
+      </c>
+      <c r="G22" s="68"/>
+      <c r="H22" s="69">
+        <f>(E22-C22)/E22</f>
+        <v>-1.7859491099447981E-3</v>
+      </c>
+      <c r="S22" s="1">
         <v>5</v>
       </c>
-      <c r="B22" s="1">
+      <c r="T22" s="1">
         <v>2011</v>
       </c>
-      <c r="C22" s="53">
+      <c r="U22" s="53">
         <v>19.042553013539081</v>
       </c>
-      <c r="D22" s="52">
+      <c r="V22" s="52">
         <v>12.486065787224014</v>
       </c>
-      <c r="E22" s="41">
+      <c r="W22" s="41">
         <f t="shared" si="1"/>
         <v>-6.5564872263150669</v>
       </c>
-      <c r="I22" s="1">
+      <c r="AA22" s="1">
         <v>4</v>
       </c>
-      <c r="J22" s="42">
+      <c r="AB22" s="42">
         <v>2015</v>
       </c>
-      <c r="K22" s="43"/>
-      <c r="L22" s="40">
+      <c r="AC22" s="43"/>
+      <c r="AD22" s="40">
         <v>64.995703601698239</v>
       </c>
-      <c r="M22" s="41">
+      <c r="AE22" s="41">
         <f t="shared" si="0"/>
         <v>64.995703601698239</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" s="1">
+    <row r="23" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A23" s="66" t="s">
+        <v>223</v>
+      </c>
+      <c r="B23" s="67">
+        <v>2012</v>
+      </c>
+      <c r="C23" s="72">
+        <v>7.7289409999999998</v>
+      </c>
+      <c r="D23" s="74">
+        <v>7.7289409999999998</v>
+      </c>
+      <c r="E23" s="75">
+        <v>5.0621119999999997E-5</v>
+      </c>
+      <c r="F23" s="68" t="s">
+        <v>230</v>
+      </c>
+      <c r="G23" s="68"/>
+      <c r="H23" s="70">
+        <f>(E23-C23)/E23</f>
+        <v>-152681.14136708158</v>
+      </c>
+      <c r="S23" s="1">
         <v>6</v>
       </c>
-      <c r="B23" s="1">
+      <c r="T23" s="1">
         <v>2011</v>
       </c>
-      <c r="C23" s="53">
+      <c r="U23" s="53">
         <v>5.5691700278829366</v>
       </c>
-      <c r="D23" s="52">
+      <c r="V23" s="52">
         <v>0.6482647808533899</v>
       </c>
-      <c r="E23" s="41">
+      <c r="W23" s="41">
         <f t="shared" si="1"/>
         <v>-4.9209052470295465</v>
       </c>
-      <c r="I23" s="1">
+      <c r="AA23" s="1">
         <v>5</v>
       </c>
-      <c r="J23" s="1">
+      <c r="AB23" s="1">
         <v>2011</v>
       </c>
-      <c r="K23" s="39">
+      <c r="AC23" s="39">
         <v>19.042553013539081</v>
       </c>
-      <c r="L23" s="40">
+      <c r="AD23" s="40">
         <v>12.486065787224014</v>
       </c>
-      <c r="M23" s="41">
+      <c r="AE23" s="41">
         <f t="shared" si="0"/>
         <v>-6.5564872263150669</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24" s="1">
+    <row r="24" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A24" s="66" t="s">
+        <v>223</v>
+      </c>
+      <c r="B24" s="67">
+        <v>2013</v>
+      </c>
+      <c r="C24" s="72">
+        <v>36.214897000000001</v>
+      </c>
+      <c r="D24" s="74">
+        <v>36.2149</v>
+      </c>
+      <c r="E24" s="74">
+        <v>36.150329999999997</v>
+      </c>
+      <c r="F24" s="68" t="s">
+        <v>230</v>
+      </c>
+      <c r="G24" s="68"/>
+      <c r="H24" s="69">
+        <f>(E24-C24)/E24</f>
+        <v>-1.7860694494352838E-3</v>
+      </c>
+      <c r="S24" s="1">
         <v>1</v>
       </c>
-      <c r="B24" s="1">
+      <c r="T24" s="1">
         <v>2012</v>
       </c>
-      <c r="C24" s="39">
+      <c r="U24" s="39">
         <v>14.430646157550678</v>
       </c>
-      <c r="D24" s="40">
+      <c r="V24" s="40">
         <v>11.148345111979213</v>
       </c>
-      <c r="E24" s="41">
+      <c r="W24" s="41">
         <f t="shared" si="1"/>
         <v>-3.2823010455714652</v>
       </c>
-      <c r="I24" s="1">
+      <c r="AA24" s="1">
         <v>5</v>
       </c>
-      <c r="J24" s="1">
+      <c r="AB24" s="1">
         <v>2012</v>
       </c>
-      <c r="K24" s="39">
+      <c r="AC24" s="39">
         <v>7.7123289901518772</v>
       </c>
-      <c r="L24" s="40">
+      <c r="AD24" s="40">
         <v>7.7289411623128679</v>
       </c>
-      <c r="M24" s="41">
+      <c r="AE24" s="41">
         <f t="shared" si="0"/>
         <v>1.6612172160990646E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" s="1">
+    <row r="25" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A25" s="66" t="s">
+        <v>223</v>
+      </c>
+      <c r="B25" s="67">
+        <v>2014</v>
+      </c>
+      <c r="C25" s="72">
+        <v>55.974493000000002</v>
+      </c>
+      <c r="D25" s="74">
+        <v>55.974493000000002</v>
+      </c>
+      <c r="E25" s="74">
+        <v>55.874690000000001</v>
+      </c>
+      <c r="F25" s="68" t="s">
+        <v>230</v>
+      </c>
+      <c r="G25" s="68"/>
+      <c r="H25" s="69">
+        <f>(E25-C25)/E25</f>
+        <v>-1.7861933551667386E-3</v>
+      </c>
+      <c r="S25" s="1">
         <v>2</v>
       </c>
-      <c r="B25" s="1">
+      <c r="T25" s="1">
         <v>2012</v>
       </c>
-      <c r="C25" s="39">
+      <c r="U25" s="39">
         <v>24.597632137224569</v>
       </c>
-      <c r="D25" s="40">
+      <c r="V25" s="40">
         <v>12.322574278492283</v>
       </c>
-      <c r="E25" s="41">
+      <c r="W25" s="41">
         <f t="shared" si="1"/>
         <v>-12.275057858732286</v>
       </c>
-      <c r="I25" s="1">
+      <c r="AA25" s="1">
         <v>5</v>
       </c>
-      <c r="J25" s="1">
+      <c r="AB25" s="1">
         <v>2013</v>
       </c>
-      <c r="K25" s="39">
+      <c r="AC25" s="39">
         <v>35.404962770162811</v>
       </c>
-      <c r="L25" s="40">
+      <c r="AD25" s="40">
         <v>36.214896617535196</v>
       </c>
-      <c r="M25" s="41">
+      <c r="AE25" s="41">
         <f t="shared" si="0"/>
         <v>0.80993384737238472</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" s="1">
-        <v>3</v>
-      </c>
-      <c r="B26" s="1">
+    <row r="26" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A26" s="66" t="s">
+        <v>223</v>
+      </c>
+      <c r="B26" s="67">
+        <v>2015</v>
+      </c>
+      <c r="C26" s="72">
+        <v>51.153748</v>
+      </c>
+      <c r="D26" s="74">
+        <v>51.153748</v>
+      </c>
+      <c r="E26" s="74">
+        <v>51.062539999999998</v>
+      </c>
+      <c r="F26" s="68" t="s">
+        <v>230</v>
+      </c>
+      <c r="G26" s="68"/>
+      <c r="H26" s="69">
+        <f>(E26-C26)/E26</f>
+        <v>-1.78620178314674E-3</v>
+      </c>
+      <c r="S26" s="1">
+        <v>3</v>
+      </c>
+      <c r="T26" s="1">
         <v>2012</v>
       </c>
-      <c r="C26" s="39">
+      <c r="U26" s="39">
         <v>4.2278309234767981</v>
       </c>
-      <c r="D26" s="40">
+      <c r="V26" s="40">
         <v>4.2925414474434866</v>
       </c>
-      <c r="E26" s="41">
+      <c r="W26" s="41">
         <f t="shared" si="1"/>
         <v>6.4710523966688527E-2</v>
       </c>
-      <c r="I26" s="1">
+      <c r="AA26" s="1">
         <v>5</v>
       </c>
-      <c r="J26" s="1">
+      <c r="AB26" s="1">
         <v>2014</v>
       </c>
-      <c r="K26" s="39">
+      <c r="AC26" s="39">
         <v>55.856430131381813</v>
       </c>
-      <c r="L26" s="40">
+      <c r="AD26" s="40">
         <v>55.974492961519047</v>
       </c>
-      <c r="M26" s="41">
+      <c r="AE26" s="41">
         <f t="shared" si="0"/>
         <v>0.11806283013723373</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A27" s="1">
+    <row r="27" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A27" s="66" t="s">
+        <v>224</v>
+      </c>
+      <c r="B27" s="67">
+        <v>2011</v>
+      </c>
+      <c r="C27" s="72">
+        <v>5.5771870000000003</v>
+      </c>
+      <c r="D27" s="75">
+        <v>5.7327260000000004</v>
+      </c>
+      <c r="E27" s="74">
+        <v>5.5672420000000002</v>
+      </c>
+      <c r="F27" s="68" t="s">
+        <v>228</v>
+      </c>
+      <c r="G27" s="68"/>
+      <c r="H27" s="69">
+        <f>(E27-C27)/E27</f>
+        <v>-1.7863423217456852E-3</v>
+      </c>
+      <c r="S27" s="1">
         <v>4</v>
       </c>
-      <c r="B27" s="1">
+      <c r="T27" s="1">
         <v>2012</v>
       </c>
-      <c r="C27" s="39">
+      <c r="U27" s="39">
         <v>5.9905108913495493</v>
       </c>
-      <c r="D27" s="40">
+      <c r="V27" s="40">
         <v>5.9977010626825571</v>
       </c>
-      <c r="E27" s="41">
+      <c r="W27" s="41">
         <f t="shared" si="1"/>
         <v>7.190171333007811E-3</v>
       </c>
-      <c r="I27" s="1">
+      <c r="AA27" s="1">
         <v>5</v>
       </c>
-      <c r="J27" s="42">
+      <c r="AB27" s="42">
         <v>2015</v>
       </c>
-      <c r="K27" s="43"/>
-      <c r="L27" s="40">
+      <c r="AC27" s="43"/>
+      <c r="AD27" s="40">
         <v>51.15374766070407</v>
       </c>
-      <c r="M27" s="41">
+      <c r="AE27" s="41">
         <f t="shared" si="0"/>
         <v>51.15374766070407</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A28" s="1">
+    <row r="28" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A28" s="66" t="s">
+        <v>224</v>
+      </c>
+      <c r="B28" s="67">
+        <v>2012</v>
+      </c>
+      <c r="C28" s="72">
+        <v>3.6994479999999998</v>
+      </c>
+      <c r="D28" s="74">
+        <v>3.6994479999999998</v>
+      </c>
+      <c r="E28" s="74">
+        <v>3.6928519999999998</v>
+      </c>
+      <c r="F28" s="68" t="s">
+        <v>228</v>
+      </c>
+      <c r="G28" s="68"/>
+      <c r="H28" s="69">
+        <f>(E28-C28)/E28</f>
+        <v>-1.7861533578925034E-3</v>
+      </c>
+      <c r="S28" s="1">
         <v>5</v>
       </c>
-      <c r="B28" s="1">
+      <c r="T28" s="1">
         <v>2012</v>
       </c>
-      <c r="C28" s="39">
+      <c r="U28" s="39">
         <v>7.7123289901518772</v>
       </c>
-      <c r="D28" s="40">
+      <c r="V28" s="40">
         <v>7.7289411623128679</v>
       </c>
-      <c r="E28" s="41">
+      <c r="W28" s="41">
         <f t="shared" si="1"/>
         <v>1.6612172160990646E-2</v>
       </c>
-      <c r="I28" s="1">
+      <c r="AA28" s="1">
         <v>6</v>
       </c>
-      <c r="J28" s="1">
+      <c r="AB28" s="1">
         <v>2011</v>
       </c>
-      <c r="K28" s="39">
+      <c r="AC28" s="39">
         <v>5.5691700278829366</v>
       </c>
-      <c r="L28" s="40">
+      <c r="AD28" s="40">
         <v>0.6482647808533899</v>
       </c>
-      <c r="M28" s="41">
+      <c r="AE28" s="41">
         <f t="shared" si="0"/>
         <v>-4.9209052470295465</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A29" s="1">
+    <row r="29" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A29" s="66" t="s">
+        <v>224</v>
+      </c>
+      <c r="B29" s="67">
+        <v>2013</v>
+      </c>
+      <c r="C29" s="72">
+        <v>16.269772</v>
+      </c>
+      <c r="D29" s="74">
+        <v>16.269770000000001</v>
+      </c>
+      <c r="E29" s="74">
+        <v>16.240760000000002</v>
+      </c>
+      <c r="F29" s="68" t="s">
+        <v>228</v>
+      </c>
+      <c r="G29" s="68"/>
+      <c r="H29" s="69">
+        <f>(E29-C29)/E29</f>
+        <v>-1.7863696033928237E-3</v>
+      </c>
+      <c r="S29" s="1">
         <v>6</v>
       </c>
-      <c r="B29" s="1">
+      <c r="T29" s="1">
         <v>2012</v>
       </c>
-      <c r="C29" s="39">
+      <c r="U29" s="39">
         <v>3.6804328118880743</v>
       </c>
-      <c r="D29" s="40">
+      <c r="V29" s="40">
         <v>3.6994482564836635</v>
       </c>
-      <c r="E29" s="41">
+      <c r="W29" s="41">
         <f t="shared" si="1"/>
         <v>1.9015444595589237E-2</v>
       </c>
-      <c r="I29" s="1">
+      <c r="AA29" s="1">
         <v>6</v>
       </c>
-      <c r="J29" s="1">
+      <c r="AB29" s="1">
         <v>2012</v>
       </c>
-      <c r="K29" s="39">
+      <c r="AC29" s="39">
         <v>3.6804328118880743</v>
       </c>
-      <c r="L29" s="40">
+      <c r="AD29" s="40">
         <v>3.6994482564836635</v>
       </c>
-      <c r="M29" s="41">
+      <c r="AE29" s="41">
         <f t="shared" si="0"/>
         <v>1.9015444595589237E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A30" s="1">
+    <row r="30" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A30" s="66" t="s">
+        <v>224</v>
+      </c>
+      <c r="B30" s="67">
+        <v>2014</v>
+      </c>
+      <c r="C30" s="72">
+        <v>13.206845</v>
+      </c>
+      <c r="D30" s="74">
+        <v>13.206845</v>
+      </c>
+      <c r="E30" s="74">
+        <v>13.183299999999999</v>
+      </c>
+      <c r="F30" s="68" t="s">
+        <v>228</v>
+      </c>
+      <c r="G30" s="68"/>
+      <c r="H30" s="69">
+        <f>(E30-C30)/E30</f>
+        <v>-1.7859716459460357E-3</v>
+      </c>
+      <c r="S30" s="1">
         <v>1</v>
       </c>
-      <c r="B30" s="1">
+      <c r="T30" s="1">
         <v>2013</v>
       </c>
-      <c r="C30" s="39">
+      <c r="U30" s="39">
         <v>24.026385480314023</v>
       </c>
-      <c r="D30" s="40">
+      <c r="V30" s="40">
         <v>20.605732597297074</v>
       </c>
-      <c r="E30" s="41">
+      <c r="W30" s="41">
         <f t="shared" si="1"/>
         <v>-3.4206528830169489</v>
       </c>
-      <c r="I30" s="1">
+      <c r="AA30" s="1">
         <v>6</v>
       </c>
-      <c r="J30" s="1">
+      <c r="AB30" s="1">
         <v>2013</v>
       </c>
-      <c r="K30" s="39">
+      <c r="AC30" s="39">
         <v>15.943018834391994</v>
       </c>
-      <c r="L30" s="40">
+      <c r="AD30" s="40">
         <v>16.269771518398983</v>
       </c>
-      <c r="M30" s="41">
+      <c r="AE30" s="41">
         <f t="shared" si="0"/>
         <v>0.32675268400698876</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A31" s="1">
+    <row r="31" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A31" s="66" t="s">
+        <v>224</v>
+      </c>
+      <c r="B31" s="67">
+        <v>2015</v>
+      </c>
+      <c r="C31" s="72">
+        <v>23.588162000000001</v>
+      </c>
+      <c r="D31" s="74">
+        <v>23.588162000000001</v>
+      </c>
+      <c r="E31" s="74">
+        <v>23.546099999999999</v>
+      </c>
+      <c r="F31" s="68" t="s">
+        <v>228</v>
+      </c>
+      <c r="G31" s="68"/>
+      <c r="H31" s="69">
+        <f>(E31-C31)/E31</f>
+        <v>-1.7863680184829495E-3</v>
+      </c>
+      <c r="S31" s="1">
         <v>2</v>
       </c>
-      <c r="B31" s="1">
+      <c r="T31" s="1">
         <v>2013</v>
       </c>
-      <c r="C31" s="39">
+      <c r="U31" s="39">
         <v>32.058157301863403</v>
       </c>
-      <c r="D31" s="40">
+      <c r="V31" s="40">
         <v>32.226103252712221</v>
       </c>
-      <c r="E31" s="41">
+      <c r="W31" s="41">
         <f t="shared" si="1"/>
         <v>0.16794595084881792</v>
       </c>
-      <c r="I31" s="1">
+      <c r="AA31" s="1">
         <v>6</v>
       </c>
-      <c r="J31" s="1">
+      <c r="AB31" s="1">
         <v>2014</v>
       </c>
-      <c r="K31" s="39">
+      <c r="AC31" s="39">
         <v>11.747938582754008</v>
       </c>
-      <c r="L31" s="40">
+      <c r="AD31" s="40">
         <v>13.206844518128886</v>
       </c>
-      <c r="M31" s="41">
+      <c r="AE31" s="41">
         <f t="shared" si="0"/>
         <v>1.4589059353748777</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A32" s="1">
-        <v>3</v>
-      </c>
-      <c r="B32" s="1">
+    <row r="32" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="S32" s="1">
+        <v>3</v>
+      </c>
+      <c r="T32" s="1">
         <v>2013</v>
       </c>
-      <c r="C32" s="39">
+      <c r="U32" s="39">
         <v>19.195853054929469</v>
       </c>
-      <c r="D32" s="40">
+      <c r="V32" s="40">
         <v>19.10728323177532</v>
       </c>
-      <c r="E32" s="41">
+      <c r="W32" s="41">
         <f t="shared" si="1"/>
         <v>-8.8569823154148963E-2</v>
       </c>
-      <c r="I32" s="42">
+      <c r="AA32" s="42">
         <v>6</v>
       </c>
-      <c r="J32" s="42">
+      <c r="AB32" s="42">
         <v>2015</v>
       </c>
-      <c r="K32" s="43"/>
-      <c r="L32" s="40">
+      <c r="AC32" s="43"/>
+      <c r="AD32" s="40">
         <v>23.588162023184807</v>
       </c>
-      <c r="M32" s="41">
+      <c r="AE32" s="41">
         <f t="shared" si="0"/>
         <v>23.588162023184807</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="1">
+    <row r="33" spans="19:24" x14ac:dyDescent="0.25">
+      <c r="S33" s="1">
         <v>4</v>
       </c>
-      <c r="B33" s="1">
+      <c r="T33" s="1">
         <v>2013</v>
       </c>
-      <c r="C33" s="39">
+      <c r="U33" s="39">
         <v>20.115441999783801</v>
       </c>
-      <c r="D33" s="40">
+      <c r="V33" s="40">
         <v>20.814663293615897</v>
       </c>
-      <c r="E33" s="41">
+      <c r="W33" s="41">
         <f t="shared" si="1"/>
         <v>0.69922129383209608</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="1">
+    <row r="34" spans="19:24" x14ac:dyDescent="0.25">
+      <c r="S34" s="1">
         <v>5</v>
       </c>
-      <c r="B34" s="1">
+      <c r="T34" s="1">
         <v>2013</v>
       </c>
-      <c r="C34" s="39">
+      <c r="U34" s="39">
         <v>35.404962770162811</v>
       </c>
-      <c r="D34" s="40">
+      <c r="V34" s="40">
         <v>36.214896617535196</v>
       </c>
-      <c r="E34" s="41">
+      <c r="W34" s="41">
         <f t="shared" si="1"/>
         <v>0.80993384737238472</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="1">
+    <row r="35" spans="19:24" x14ac:dyDescent="0.25">
+      <c r="S35" s="1">
         <v>6</v>
       </c>
-      <c r="B35" s="1">
+      <c r="T35" s="1">
         <v>2013</v>
       </c>
-      <c r="C35" s="39">
+      <c r="U35" s="39">
         <v>15.943018834391994</v>
       </c>
-      <c r="D35" s="40">
+      <c r="V35" s="40">
         <v>16.269771518398983</v>
       </c>
-      <c r="E35" s="41">
+      <c r="W35" s="41">
         <f t="shared" si="1"/>
         <v>0.32675268400698876</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="1">
+    <row r="36" spans="19:24" x14ac:dyDescent="0.25">
+      <c r="S36" s="1">
         <v>1</v>
       </c>
-      <c r="B36" s="1">
+      <c r="T36" s="1">
         <v>2014</v>
       </c>
-      <c r="C36" s="39">
+      <c r="U36" s="39">
         <v>30.282252255810182</v>
       </c>
-      <c r="D36" s="40">
+      <c r="V36" s="40">
         <v>21.997187461853823</v>
       </c>
-      <c r="E36" s="41">
+      <c r="W36" s="41">
         <f t="shared" si="1"/>
         <v>-8.2850647939563586</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="1">
+    <row r="37" spans="19:24" x14ac:dyDescent="0.25">
+      <c r="S37" s="1">
         <v>2</v>
       </c>
-      <c r="B37" s="1">
+      <c r="T37" s="1">
         <v>2014</v>
       </c>
-      <c r="C37" s="39">
+      <c r="U37" s="39">
         <v>56.843162018861399</v>
       </c>
-      <c r="D37" s="40">
+      <c r="V37" s="40">
         <v>59.143658115801664</v>
       </c>
-      <c r="E37" s="41">
+      <c r="W37" s="41">
         <f t="shared" si="1"/>
         <v>2.3004960969402646</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="1">
-        <v>3</v>
-      </c>
-      <c r="B38" s="1">
+    <row r="38" spans="19:24" x14ac:dyDescent="0.25">
+      <c r="S38" s="1">
+        <v>3</v>
+      </c>
+      <c r="T38" s="1">
         <v>2014</v>
       </c>
-      <c r="C38" s="39">
+      <c r="U38" s="39">
         <v>16.51317404346857</v>
       </c>
-      <c r="D38" s="40">
+      <c r="V38" s="40">
         <v>6.4460640319366291</v>
       </c>
-      <c r="E38" s="41">
+      <c r="W38" s="41">
         <f t="shared" si="1"/>
         <v>-10.067110011531941</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="1">
+    <row r="39" spans="19:24" x14ac:dyDescent="0.25">
+      <c r="S39" s="1">
         <v>4</v>
       </c>
-      <c r="B39" s="1">
+      <c r="T39" s="1">
         <v>2014</v>
       </c>
-      <c r="C39" s="39">
+      <c r="U39" s="39">
         <v>15.567517404912163</v>
       </c>
-      <c r="D39" s="40">
+      <c r="V39" s="40">
         <v>15.617248728120618</v>
       </c>
-      <c r="E39" s="41">
+      <c r="W39" s="41">
         <f t="shared" si="1"/>
         <v>4.973132320845508E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="1">
+    <row r="40" spans="19:24" x14ac:dyDescent="0.25">
+      <c r="S40" s="1">
         <v>5</v>
       </c>
-      <c r="B40" s="1">
+      <c r="T40" s="1">
         <v>2014</v>
       </c>
-      <c r="C40" s="39">
+      <c r="U40" s="39">
         <v>55.856430131381813</v>
       </c>
-      <c r="D40" s="40">
+      <c r="V40" s="40">
         <v>55.974492961519047</v>
       </c>
-      <c r="E40" s="41">
+      <c r="W40" s="41">
         <f t="shared" si="1"/>
         <v>0.11806283013723373</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="1">
+    <row r="41" spans="19:24" x14ac:dyDescent="0.25">
+      <c r="S41" s="1">
         <v>6</v>
       </c>
-      <c r="B41" s="1">
+      <c r="T41" s="1">
         <v>2014</v>
       </c>
-      <c r="C41" s="39">
+      <c r="U41" s="39">
         <v>11.747938582754008</v>
       </c>
-      <c r="D41" s="40">
+      <c r="V41" s="40">
         <v>13.206844518128886</v>
       </c>
-      <c r="E41" s="41">
+      <c r="W41" s="41">
         <f t="shared" si="1"/>
         <v>1.4589059353748777</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="42">
+    <row r="42" spans="19:24" x14ac:dyDescent="0.25">
+      <c r="S42" s="42">
         <v>1</v>
       </c>
-      <c r="B42" s="42">
+      <c r="T42" s="42">
         <v>2015</v>
       </c>
-      <c r="C42" s="43"/>
-      <c r="D42" s="40">
+      <c r="U42" s="43"/>
+      <c r="V42" s="40">
         <v>6.4732370062486293</v>
       </c>
-      <c r="E42" s="41">
+      <c r="W42" s="41">
         <f t="shared" si="1"/>
         <v>6.4732370062486293</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="1">
+    <row r="43" spans="19:24" x14ac:dyDescent="0.25">
+      <c r="S43" s="1">
         <v>2</v>
       </c>
-      <c r="B43" s="42">
+      <c r="T43" s="42">
         <v>2015</v>
       </c>
-      <c r="C43" s="43"/>
-      <c r="D43" s="40">
+      <c r="U43" s="43"/>
+      <c r="V43" s="40">
         <v>14.899464757295986</v>
       </c>
-      <c r="E43" s="41">
+      <c r="W43" s="41">
         <f t="shared" si="1"/>
         <v>14.899464757295986</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="1">
-        <v>3</v>
-      </c>
-      <c r="B44" s="42">
+    <row r="44" spans="19:24" x14ac:dyDescent="0.25">
+      <c r="S44" s="1">
+        <v>3</v>
+      </c>
+      <c r="T44" s="42">
         <v>2015</v>
       </c>
-      <c r="C44" s="43"/>
-      <c r="D44" s="40">
+      <c r="U44" s="43"/>
+      <c r="V44" s="40">
         <v>10.609299296662067</v>
       </c>
-      <c r="E44" s="41">
+      <c r="W44" s="41">
         <f t="shared" si="1"/>
         <v>10.609299296662067</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="1">
+    <row r="45" spans="19:24" x14ac:dyDescent="0.25">
+      <c r="S45" s="1">
         <v>4</v>
       </c>
-      <c r="B45" s="42">
+      <c r="T45" s="42">
         <v>2015</v>
       </c>
-      <c r="C45" s="43"/>
-      <c r="D45" s="52">
+      <c r="U45" s="43"/>
+      <c r="V45" s="52">
         <v>64.995703601698239</v>
       </c>
-      <c r="E45" s="41">
+      <c r="W45" s="41">
         <f t="shared" si="1"/>
         <v>64.995703601698239</v>
       </c>
-      <c r="F45" s="55">
+      <c r="X45" s="55">
         <v>9.9700000000000006</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="1">
+    <row r="46" spans="19:24" x14ac:dyDescent="0.25">
+      <c r="S46" s="1">
         <v>5</v>
       </c>
-      <c r="B46" s="42">
+      <c r="T46" s="42">
         <v>2015</v>
       </c>
-      <c r="C46" s="43"/>
-      <c r="D46" s="40">
+      <c r="U46" s="43"/>
+      <c r="V46" s="40">
         <v>51.15374766070407</v>
       </c>
-      <c r="E46" s="41">
+      <c r="W46" s="41">
         <f t="shared" si="1"/>
         <v>51.15374766070407</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="42">
+    <row r="47" spans="19:24" x14ac:dyDescent="0.25">
+      <c r="S47" s="42">
         <v>6</v>
       </c>
-      <c r="B47" s="42">
+      <c r="T47" s="42">
         <v>2015</v>
       </c>
-      <c r="C47" s="43"/>
-      <c r="D47" s="40">
+      <c r="U47" s="43"/>
+      <c r="V47" s="40">
         <v>23.588162023184807</v>
       </c>
-      <c r="E47" s="41">
+      <c r="W47" s="41">
         <f t="shared" si="1"/>
         <v>23.588162023184807</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A16:E47">
+  <autoFilter ref="S16:W47">
     <filterColumn colId="2" showButton="0"/>
     <filterColumn colId="3" showButton="0"/>
   </autoFilter>
   <mergeCells count="3">
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="U16:W16"/>
+    <mergeCell ref="S16:S17"/>
+    <mergeCell ref="T16:T17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
a bunch of changes
</commit_message>
<xml_diff>
--- a/Data/flow/NO3-N Loss.xlsx
+++ b/Data/flow/NO3-N Loss.xlsx
@@ -24,6 +24,8 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">rotations!$A$1:$H$63</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">SERF!$S$16:$W$47</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sites!$A$2:$D$2</definedName>
+    <definedName name="N_Load_yearly_SERF_IA" localSheetId="3">SERF!$J$1:$P$11</definedName>
+    <definedName name="N_Load_yearly_SERF_IA_1" localSheetId="3">SERF!$A$35:$G$45</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <pivotCaches>
@@ -37,8 +39,52 @@
 </workbook>
 </file>
 
+<file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <connection id="1" name="N_Load_yearly_SERF_IA" type="6" refreshedVersion="5" background="1" saveData="1">
+    <textPr codePage="437" sourceFile="C:\Users\gio\Google Drive\MODELLING\SERF_IA\N_Load_yearly_SERF_IA.prn">
+      <textFields count="7">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="2" name="N_Load_yearly_SERF_IA1" type="6" refreshedVersion="5" background="1">
+    <textPr codePage="437" sourceFile="C:\Users\gio\Google Drive\MODELLING\SERF_IA\N_Load_yearly_SERF_IA.prn">
+      <textFields count="7">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="3" name="N_Load_yearly_SERF_IA2" type="6" refreshedVersion="5" background="1" saveData="1">
+    <textPr codePage="437" sourceFile="C:\Users\gio\Google Drive\MODELLING\SERF_IA\N_Load_yearly_SERF_IA.prn">
+      <textFields count="7">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+</connections>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4737" uniqueCount="440">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4751" uniqueCount="447">
   <si>
     <t>Key</t>
   </si>
@@ -1359,6 +1405,27 @@
   <si>
     <t>MANAGE</t>
   </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>S1</t>
+  </si>
+  <si>
+    <t>S2</t>
+  </si>
+  <si>
+    <t>S3</t>
+  </si>
+  <si>
+    <t>S4</t>
+  </si>
+  <si>
+    <t>S5</t>
+  </si>
+  <si>
+    <t>S6</t>
+  </si>
 </sst>
 </file>
 
@@ -1670,7 +1737,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -1855,6 +1922,22 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2201,6 +2284,14 @@
 </pivotTableDefinition>
 </file>
 
+<file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="N_Load_yearly_SERF_IA_1" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="N_Load_yearly_SERF_IA" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2467,8 +2558,8 @@
   <dimension ref="A1:I1023"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I34" sqref="I34"/>
+      <pane ySplit="1" topLeftCell="A230" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2538,9 +2629,9 @@
         <f>Data!E2</f>
         <v>2011</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="56">
         <f>Data!F2</f>
-        <v>9.1024758000000006</v>
+        <v>9.1025996493385506</v>
       </c>
       <c r="G2" s="24">
         <f>Data!K2</f>
@@ -2575,9 +2666,9 @@
         <f>Data!E3</f>
         <v>2011</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="56">
         <f>Data!F3</f>
-        <v>42.465522999999997</v>
+        <v>30.2445924049733</v>
       </c>
       <c r="G3" s="24">
         <f>Data!K3</f>
@@ -2612,9 +2703,9 @@
         <f>Data!E4</f>
         <v>2011</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="56">
         <f>Data!F4</f>
-        <v>11.357567</v>
+        <v>9.7001828208000003</v>
       </c>
       <c r="G4" s="24">
         <f>Data!K4</f>
@@ -2649,9 +2740,9 @@
         <f>Data!E5</f>
         <v>2011</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="56">
         <f>Data!F5</f>
-        <v>10.164596</v>
+        <v>9.5913074339377609</v>
       </c>
       <c r="G5" s="24">
         <f>Data!K5</f>
@@ -2686,9 +2777,9 @@
         <f>Data!E6</f>
         <v>2011</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="56">
         <f>Data!F6</f>
-        <v>24.493995999999999</v>
+        <v>19.05049434675</v>
       </c>
       <c r="G6" s="24">
         <f>Data!K6</f>
@@ -2723,9 +2814,9 @@
         <f>Data!E7</f>
         <v>2011</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="56">
         <f>Data!F7</f>
-        <v>5.7327260000000004</v>
+        <v>5.5771901070694296</v>
       </c>
       <c r="G7" s="24">
         <f>Data!K7</f>
@@ -2760,9 +2851,9 @@
         <f>Data!E8</f>
         <v>2012</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="56">
         <f>Data!F8</f>
-        <v>14.461128199999999</v>
+        <v>14.461191714423901</v>
       </c>
       <c r="G8" s="24">
         <f>Data!K8</f>
@@ -2797,9 +2888,9 @@
         <f>Data!E9</f>
         <v>2012</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="56">
         <f>Data!F9</f>
-        <v>12.322573999999999</v>
+        <v>12.322867652470499</v>
       </c>
       <c r="G9" s="24">
         <f>Data!K9</f>
@@ -2834,9 +2925,9 @@
         <f>Data!E10</f>
         <v>2012</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="56">
         <f>Data!F10</f>
-        <v>4.2925409999999999</v>
+        <v>4.2925759112617303</v>
       </c>
       <c r="G10" s="24">
         <f>Data!K10</f>
@@ -2871,9 +2962,9 @@
         <f>Data!E11</f>
         <v>2012</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="56">
         <f>Data!F11</f>
-        <v>5.9977010000000002</v>
+        <v>5.9977010626825402</v>
       </c>
       <c r="G11" s="24">
         <f>Data!K11</f>
@@ -2908,9 +2999,9 @@
         <f>Data!E12</f>
         <v>2012</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="56">
         <f>Data!F12</f>
-        <v>7.7289409999999998</v>
+        <v>7.7289606995984901</v>
       </c>
       <c r="G12" s="24">
         <f>Data!K12</f>
@@ -2945,9 +3036,9 @@
         <f>Data!E13</f>
         <v>2012</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="56">
         <f>Data!F13</f>
-        <v>3.6994479999999998</v>
+        <v>3.6994482564836701</v>
       </c>
       <c r="G13" s="24">
         <f>Data!K13</f>
@@ -2982,9 +3073,9 @@
         <f>Data!E14</f>
         <v>2013</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="56">
         <f>Data!F14</f>
-        <v>23.890933</v>
+        <v>23.8985946874608</v>
       </c>
       <c r="G14" s="24">
         <f>Data!K14</f>
@@ -3019,9 +3110,9 @@
         <f>Data!E15</f>
         <v>2013</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="56">
         <f>Data!F15</f>
-        <v>32.226100000000002</v>
+        <v>32.235161800374001</v>
       </c>
       <c r="G15" s="24">
         <f>Data!K15</f>
@@ -3056,9 +3147,9 @@
         <f>Data!E16</f>
         <v>2013</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="56">
         <f>Data!F16</f>
-        <v>19.107279999999999</v>
+        <v>19.1132729249378</v>
       </c>
       <c r="G16" s="24">
         <f>Data!K16</f>
@@ -3093,9 +3184,9 @@
         <f>Data!E17</f>
         <v>2013</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="56">
         <f>Data!F17</f>
-        <v>20.81466</v>
+        <v>20.819684091088099</v>
       </c>
       <c r="G17" s="24">
         <f>Data!K17</f>
@@ -3130,9 +3221,9 @@
         <f>Data!E18</f>
         <v>2013</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="56">
         <f>Data!F18</f>
-        <v>36.2149</v>
+        <v>36.226840773504399</v>
       </c>
       <c r="G18" s="24">
         <f>Data!K18</f>
@@ -3167,9 +3258,9 @@
         <f>Data!E19</f>
         <v>2013</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="56">
         <f>Data!F19</f>
-        <v>16.269770000000001</v>
+        <v>16.271459630304602</v>
       </c>
       <c r="G19" s="24">
         <f>Data!K19</f>
@@ -3204,9 +3295,9 @@
         <f>Data!E20</f>
         <v>2014</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="56">
         <f>Data!F20</f>
-        <v>37.126836699999998</v>
+        <v>37.154274293639098</v>
       </c>
       <c r="G20" s="24">
         <f>Data!K20</f>
@@ -3241,9 +3332,9 @@
         <f>Data!E21</f>
         <v>2014</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="56">
         <f>Data!F21</f>
-        <v>59.143658000000002</v>
+        <v>59.172386135875797</v>
       </c>
       <c r="G21" s="24">
         <f>Data!K21</f>
@@ -3278,9 +3369,9 @@
         <f>Data!E22</f>
         <v>2014</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="56">
         <f>Data!F22</f>
-        <v>6.4460639999999998</v>
+        <v>6.4707712039542704</v>
       </c>
       <c r="G22" s="24">
         <f>Data!K22</f>
@@ -3315,9 +3406,9 @@
         <f>Data!E23</f>
         <v>2014</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="56">
         <f>Data!F23</f>
-        <v>15.617248999999999</v>
+        <v>15.6447669866408</v>
       </c>
       <c r="G23" s="24">
         <f>Data!K23</f>
@@ -3352,9 +3443,9 @@
         <f>Data!E24</f>
         <v>2014</v>
       </c>
-      <c r="F24">
+      <c r="F24" s="56">
         <f>Data!F24</f>
-        <v>55.974493000000002</v>
+        <v>56.005994075571202</v>
       </c>
       <c r="G24" s="24">
         <f>Data!K24</f>
@@ -3389,9 +3480,9 @@
         <f>Data!E25</f>
         <v>2014</v>
       </c>
-      <c r="F25">
+      <c r="F25" s="56">
         <f>Data!F25</f>
-        <v>13.206845</v>
+        <v>13.224573919535301</v>
       </c>
       <c r="G25" s="24">
         <f>Data!K25</f>
@@ -3426,9 +3517,9 @@
         <f>Data!E26</f>
         <v>2015</v>
       </c>
-      <c r="F26">
+      <c r="F26" s="56">
         <f>Data!F26</f>
-        <v>10.623893900000001</v>
+        <v>10.6238939286857</v>
       </c>
       <c r="G26" s="24">
         <f>Data!K26</f>
@@ -3463,9 +3554,9 @@
         <f>Data!E27</f>
         <v>2015</v>
       </c>
-      <c r="F27">
+      <c r="F27" s="56">
         <f>Data!F27</f>
-        <v>14.899558000000001</v>
+        <v>14.9004345219195</v>
       </c>
       <c r="G27" s="24">
         <f>Data!K27</f>
@@ -3500,9 +3591,9 @@
         <f>Data!E28</f>
         <v>2015</v>
       </c>
-      <c r="F28">
+      <c r="F28" s="56">
         <f>Data!F28</f>
-        <v>10.612791</v>
+        <v>10.6102212874851</v>
       </c>
       <c r="G28" s="24">
         <f>Data!K28</f>
@@ -3537,9 +3628,9 @@
         <f>Data!E29</f>
         <v>2015</v>
       </c>
-      <c r="F29">
+      <c r="F29" s="56">
         <f>Data!F29</f>
-        <v>9.9698910000000005</v>
+        <v>9.9696464002593608</v>
       </c>
       <c r="G29" s="24">
         <f>Data!K29</f>
@@ -3574,9 +3665,9 @@
         <f>Data!E30</f>
         <v>2015</v>
       </c>
-      <c r="F30">
+      <c r="F30" s="56">
         <f>Data!F30</f>
-        <v>51.153748</v>
+        <v>51.166072198054799</v>
       </c>
       <c r="G30" s="24">
         <f>Data!K30</f>
@@ -3611,9 +3702,9 @@
         <f>Data!E31</f>
         <v>2015</v>
       </c>
-      <c r="F31">
+      <c r="F31" s="56">
         <f>Data!F31</f>
-        <v>23.588162000000001</v>
+        <v>23.589501119907499</v>
       </c>
       <c r="G31" s="24">
         <f>Data!K31</f>
@@ -40664,11 +40755,11 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:L1023"/>
+  <dimension ref="A1:N1023"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H19" sqref="H19"/>
+      <pane ySplit="1" topLeftCell="A227" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -40684,7 +40775,7 @@
     <col min="15" max="17" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="14" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" s="14" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>230</v>
       </c>
@@ -40722,7 +40813,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>231</v>
       </c>
@@ -40739,7 +40830,7 @@
         <v>2011</v>
       </c>
       <c r="F2" s="56">
-        <v>9.1024758000000006</v>
+        <v>9.1025996493385506</v>
       </c>
       <c r="G2">
         <v>1</v>
@@ -40759,8 +40850,14 @@
       <c r="L2">
         <v>-91.482900000000001</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M2" s="83">
+        <v>9.1025996493385506</v>
+      </c>
+      <c r="N2" s="56">
+        <v>9.1024758000000006</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>231</v>
       </c>
@@ -40777,7 +40874,7 @@
         <v>2011</v>
       </c>
       <c r="F3" s="49">
-        <v>42.465522999999997</v>
+        <v>30.2445924049733</v>
       </c>
       <c r="G3">
         <v>2</v>
@@ -40797,8 +40894,14 @@
       <c r="L3">
         <v>-91.482900000000001</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M3" s="83">
+        <v>30.2445924049733</v>
+      </c>
+      <c r="N3" s="49">
+        <v>42.465522999999997</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>231</v>
       </c>
@@ -40815,7 +40918,7 @@
         <v>2011</v>
       </c>
       <c r="F4" s="49">
-        <v>11.357567</v>
+        <v>9.7001828208000003</v>
       </c>
       <c r="G4">
         <v>3</v>
@@ -40835,8 +40938,14 @@
       <c r="L4">
         <v>-91.482900000000001</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M4" s="83">
+        <v>9.7001828208000003</v>
+      </c>
+      <c r="N4" s="49">
+        <v>11.357567</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>231</v>
       </c>
@@ -40853,7 +40962,7 @@
         <v>2011</v>
       </c>
       <c r="F5" s="49">
-        <v>10.164596</v>
+        <v>9.5913074339377609</v>
       </c>
       <c r="G5">
         <v>4</v>
@@ -40873,8 +40982,14 @@
       <c r="L5">
         <v>-91.482900000000001</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M5" s="83">
+        <v>9.5913074339377609</v>
+      </c>
+      <c r="N5" s="49">
+        <v>10.164596</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>231</v>
       </c>
@@ -40891,7 +41006,7 @@
         <v>2011</v>
       </c>
       <c r="F6" s="49">
-        <v>24.493995999999999</v>
+        <v>19.05049434675</v>
       </c>
       <c r="G6">
         <v>5</v>
@@ -40911,8 +41026,14 @@
       <c r="L6">
         <v>-91.482900000000001</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M6" s="84">
+        <v>19.05049434675</v>
+      </c>
+      <c r="N6" s="49">
+        <v>24.493995999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>231</v>
       </c>
@@ -40929,7 +41050,7 @@
         <v>2011</v>
       </c>
       <c r="F7" s="49">
-        <v>5.7327260000000004</v>
+        <v>5.5771901070694296</v>
       </c>
       <c r="G7">
         <v>6</v>
@@ -40949,8 +41070,14 @@
       <c r="L7">
         <v>-91.482900000000001</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M7" s="84">
+        <v>5.5771901070694296</v>
+      </c>
+      <c r="N7" s="49">
+        <v>5.7327260000000004</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>231</v>
       </c>
@@ -40967,7 +41094,7 @@
         <v>2012</v>
       </c>
       <c r="F8" s="56">
-        <v>14.461128199999999</v>
+        <v>14.461191714423901</v>
       </c>
       <c r="K8">
         <v>41.193800000000003</v>
@@ -40975,8 +41102,14 @@
       <c r="L8">
         <v>-91.482900000000001</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M8" s="83">
+        <v>14.461191714423901</v>
+      </c>
+      <c r="N8" s="56">
+        <v>14.461128199999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>231</v>
       </c>
@@ -40993,7 +41126,7 @@
         <v>2012</v>
       </c>
       <c r="F9" s="56">
-        <v>12.322573999999999</v>
+        <v>12.322867652470499</v>
       </c>
       <c r="K9">
         <v>41.193800000000003</v>
@@ -41001,8 +41134,14 @@
       <c r="L9">
         <v>-91.482900000000001</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M9" s="83">
+        <v>12.322867652470499</v>
+      </c>
+      <c r="N9" s="56">
+        <v>12.322573999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>231</v>
       </c>
@@ -41019,7 +41158,7 @@
         <v>2012</v>
       </c>
       <c r="F10" s="56">
-        <v>4.2925409999999999</v>
+        <v>4.2925759112617303</v>
       </c>
       <c r="K10">
         <v>41.193800000000003</v>
@@ -41027,8 +41166,14 @@
       <c r="L10">
         <v>-91.482900000000001</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M10" s="83">
+        <v>4.2925759112617303</v>
+      </c>
+      <c r="N10" s="56">
+        <v>4.2925409999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>231</v>
       </c>
@@ -41045,7 +41190,7 @@
         <v>2012</v>
       </c>
       <c r="F11" s="56">
-        <v>5.9977010000000002</v>
+        <v>5.9977010626825402</v>
       </c>
       <c r="K11">
         <v>41.193800000000003</v>
@@ -41053,8 +41198,14 @@
       <c r="L11">
         <v>-91.482900000000001</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M11" s="83">
+        <v>5.9977010626825402</v>
+      </c>
+      <c r="N11" s="56">
+        <v>5.9977010000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>231</v>
       </c>
@@ -41071,7 +41222,7 @@
         <v>2012</v>
       </c>
       <c r="F12" s="56">
-        <v>7.7289409999999998</v>
+        <v>7.7289606995984901</v>
       </c>
       <c r="K12">
         <v>41.193800000000003</v>
@@ -41079,8 +41230,14 @@
       <c r="L12">
         <v>-91.482900000000001</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M12" s="84">
+        <v>7.7289606995984901</v>
+      </c>
+      <c r="N12" s="56">
+        <v>7.7289409999999998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>231</v>
       </c>
@@ -41097,7 +41254,7 @@
         <v>2012</v>
       </c>
       <c r="F13" s="56">
-        <v>3.6994479999999998</v>
+        <v>3.6994482564836701</v>
       </c>
       <c r="K13">
         <v>41.193800000000003</v>
@@ -41105,8 +41262,14 @@
       <c r="L13">
         <v>-91.482900000000001</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M13" s="84">
+        <v>3.6994482564836701</v>
+      </c>
+      <c r="N13" s="56">
+        <v>3.6994479999999998</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>231</v>
       </c>
@@ -41123,7 +41286,7 @@
         <v>2013</v>
       </c>
       <c r="F14" s="56">
-        <v>23.890933</v>
+        <v>23.8985946874608</v>
       </c>
       <c r="K14">
         <v>41.193800000000003</v>
@@ -41131,8 +41294,14 @@
       <c r="L14">
         <v>-91.482900000000001</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M14" s="83">
+        <v>23.8985946874608</v>
+      </c>
+      <c r="N14" s="56">
+        <v>23.890933</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>231</v>
       </c>
@@ -41149,7 +41318,7 @@
         <v>2013</v>
       </c>
       <c r="F15" s="56">
-        <v>32.226100000000002</v>
+        <v>32.235161800374001</v>
       </c>
       <c r="K15">
         <v>41.193800000000003</v>
@@ -41157,8 +41326,14 @@
       <c r="L15">
         <v>-91.482900000000001</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M15" s="83">
+        <v>32.235161800374001</v>
+      </c>
+      <c r="N15" s="56">
+        <v>32.226100000000002</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>231</v>
       </c>
@@ -41175,7 +41350,7 @@
         <v>2013</v>
       </c>
       <c r="F16" s="56">
-        <v>19.107279999999999</v>
+        <v>19.1132729249378</v>
       </c>
       <c r="K16">
         <v>41.193800000000003</v>
@@ -41183,8 +41358,14 @@
       <c r="L16">
         <v>-91.482900000000001</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M16" s="83">
+        <v>19.1132729249378</v>
+      </c>
+      <c r="N16" s="56">
+        <v>19.107279999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>231</v>
       </c>
@@ -41201,7 +41382,7 @@
         <v>2013</v>
       </c>
       <c r="F17" s="56">
-        <v>20.81466</v>
+        <v>20.819684091088099</v>
       </c>
       <c r="K17">
         <v>41.193800000000003</v>
@@ -41209,8 +41390,14 @@
       <c r="L17">
         <v>-91.482900000000001</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M17" s="83">
+        <v>20.819684091088099</v>
+      </c>
+      <c r="N17" s="56">
+        <v>20.81466</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>231</v>
       </c>
@@ -41227,7 +41414,7 @@
         <v>2013</v>
       </c>
       <c r="F18" s="56">
-        <v>36.2149</v>
+        <v>36.226840773504399</v>
       </c>
       <c r="K18">
         <v>41.193800000000003</v>
@@ -41235,8 +41422,14 @@
       <c r="L18">
         <v>-91.482900000000001</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M18" s="84">
+        <v>36.226840773504399</v>
+      </c>
+      <c r="N18" s="56">
+        <v>36.2149</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>231</v>
       </c>
@@ -41253,7 +41446,7 @@
         <v>2013</v>
       </c>
       <c r="F19" s="56">
-        <v>16.269770000000001</v>
+        <v>16.271459630304602</v>
       </c>
       <c r="K19">
         <v>41.193800000000003</v>
@@ -41261,8 +41454,14 @@
       <c r="L19">
         <v>-91.482900000000001</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M19" s="84">
+        <v>16.271459630304602</v>
+      </c>
+      <c r="N19" s="56">
+        <v>16.269770000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>231</v>
       </c>
@@ -41279,7 +41478,7 @@
         <v>2014</v>
       </c>
       <c r="F20" s="56">
-        <v>37.126836699999998</v>
+        <v>37.154274293639098</v>
       </c>
       <c r="K20">
         <v>41.193800000000003</v>
@@ -41287,8 +41486,14 @@
       <c r="L20">
         <v>-91.482900000000001</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M20" s="83">
+        <v>37.154274293639098</v>
+      </c>
+      <c r="N20" s="56">
+        <v>37.126836699999998</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>231</v>
       </c>
@@ -41305,7 +41510,7 @@
         <v>2014</v>
       </c>
       <c r="F21" s="56">
-        <v>59.143658000000002</v>
+        <v>59.172386135875797</v>
       </c>
       <c r="K21">
         <v>41.193800000000003</v>
@@ -41313,8 +41518,14 @@
       <c r="L21">
         <v>-91.482900000000001</v>
       </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M21" s="83">
+        <v>59.172386135875797</v>
+      </c>
+      <c r="N21" s="56">
+        <v>59.143658000000002</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>231</v>
       </c>
@@ -41331,7 +41542,7 @@
         <v>2014</v>
       </c>
       <c r="F22" s="56">
-        <v>6.4460639999999998</v>
+        <v>6.4707712039542704</v>
       </c>
       <c r="K22">
         <v>41.193800000000003</v>
@@ -41339,8 +41550,14 @@
       <c r="L22">
         <v>-91.482900000000001</v>
       </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M22" s="83">
+        <v>6.4707712039542704</v>
+      </c>
+      <c r="N22" s="56">
+        <v>6.4460639999999998</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>231</v>
       </c>
@@ -41357,7 +41574,7 @@
         <v>2014</v>
       </c>
       <c r="F23" s="56">
-        <v>15.617248999999999</v>
+        <v>15.6447669866408</v>
       </c>
       <c r="K23">
         <v>41.193800000000003</v>
@@ -41365,8 +41582,14 @@
       <c r="L23">
         <v>-91.482900000000001</v>
       </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M23" s="83">
+        <v>15.6447669866408</v>
+      </c>
+      <c r="N23" s="56">
+        <v>15.617248999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>231</v>
       </c>
@@ -41383,7 +41606,7 @@
         <v>2014</v>
       </c>
       <c r="F24" s="56">
-        <v>55.974493000000002</v>
+        <v>56.005994075571202</v>
       </c>
       <c r="K24">
         <v>41.193800000000003</v>
@@ -41391,8 +41614,14 @@
       <c r="L24">
         <v>-91.482900000000001</v>
       </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M24" s="84">
+        <v>56.005994075571202</v>
+      </c>
+      <c r="N24" s="56">
+        <v>55.974493000000002</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>231</v>
       </c>
@@ -41409,7 +41638,7 @@
         <v>2014</v>
       </c>
       <c r="F25" s="56">
-        <v>13.206845</v>
+        <v>13.224573919535301</v>
       </c>
       <c r="K25">
         <v>41.193800000000003</v>
@@ -41417,8 +41646,14 @@
       <c r="L25">
         <v>-91.482900000000001</v>
       </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M25" s="84">
+        <v>13.224573919535301</v>
+      </c>
+      <c r="N25" s="56">
+        <v>13.206845</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>231</v>
       </c>
@@ -41435,7 +41670,7 @@
         <v>2015</v>
       </c>
       <c r="F26" s="56">
-        <v>10.623893900000001</v>
+        <v>10.6238939286857</v>
       </c>
       <c r="K26">
         <v>41.193800000000003</v>
@@ -41443,8 +41678,14 @@
       <c r="L26">
         <v>-91.482900000000001</v>
       </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M26" s="83">
+        <v>10.6238939286857</v>
+      </c>
+      <c r="N26" s="56">
+        <v>10.623893900000001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>231</v>
       </c>
@@ -41461,7 +41702,7 @@
         <v>2015</v>
       </c>
       <c r="F27" s="56">
-        <v>14.899558000000001</v>
+        <v>14.9004345219195</v>
       </c>
       <c r="K27">
         <v>41.193800000000003</v>
@@ -41469,8 +41710,14 @@
       <c r="L27">
         <v>-91.482900000000001</v>
       </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M27" s="83">
+        <v>14.9004345219195</v>
+      </c>
+      <c r="N27" s="56">
+        <v>14.899558000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>231</v>
       </c>
@@ -41487,7 +41734,7 @@
         <v>2015</v>
       </c>
       <c r="F28" s="56">
-        <v>10.612791</v>
+        <v>10.6102212874851</v>
       </c>
       <c r="K28">
         <v>41.193800000000003</v>
@@ -41495,8 +41742,14 @@
       <c r="L28">
         <v>-91.482900000000001</v>
       </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M28" s="83">
+        <v>10.6102212874851</v>
+      </c>
+      <c r="N28" s="56">
+        <v>10.612791</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>231</v>
       </c>
@@ -41513,7 +41766,7 @@
         <v>2015</v>
       </c>
       <c r="F29" s="56">
-        <v>9.9698910000000005</v>
+        <v>9.9696464002593608</v>
       </c>
       <c r="K29">
         <v>41.193800000000003</v>
@@ -41521,8 +41774,14 @@
       <c r="L29">
         <v>-91.482900000000001</v>
       </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M29" s="83">
+        <v>9.9696464002593608</v>
+      </c>
+      <c r="N29" s="56">
+        <v>9.9698910000000005</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>231</v>
       </c>
@@ -41539,7 +41798,7 @@
         <v>2015</v>
       </c>
       <c r="F30" s="56">
-        <v>51.153748</v>
+        <v>51.166072198054799</v>
       </c>
       <c r="K30">
         <v>41.193800000000003</v>
@@ -41547,8 +41806,14 @@
       <c r="L30">
         <v>-91.482900000000001</v>
       </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M30" s="84">
+        <v>51.166072198054799</v>
+      </c>
+      <c r="N30" s="56">
+        <v>51.153748</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>231</v>
       </c>
@@ -41565,7 +41830,7 @@
         <v>2015</v>
       </c>
       <c r="F31" s="56">
-        <v>23.588162000000001</v>
+        <v>23.589501119907499</v>
       </c>
       <c r="K31">
         <v>41.193800000000003</v>
@@ -41573,8 +41838,14 @@
       <c r="L31">
         <v>-91.482900000000001</v>
       </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M31" s="84">
+        <v>23.589501119907499</v>
+      </c>
+      <c r="N31" s="56">
+        <v>23.588162000000001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>232</v>
       </c>
@@ -41605,8 +41876,11 @@
       <c r="L32">
         <v>-92.196700000000007</v>
       </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M32" s="83">
+        <v>9.3818217310323497</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>232</v>
       </c>
@@ -41637,8 +41911,11 @@
       <c r="L33">
         <v>-92.196700000000007</v>
       </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M33" s="83">
+        <v>14.7041876082792</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>232</v>
       </c>
@@ -41669,8 +41946,11 @@
       <c r="L34">
         <v>-92.196700000000007</v>
       </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M34" s="83">
+        <v>3.3268933406616301</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>232</v>
       </c>
@@ -41701,8 +41981,11 @@
       <c r="L35">
         <v>-92.196700000000007</v>
       </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M35" s="83">
+        <v>1.3664545382970901</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>232</v>
       </c>
@@ -41733,8 +42016,11 @@
       <c r="L36">
         <v>-92.196700000000007</v>
       </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M36" s="84">
+        <v>20.138381222186901</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>232</v>
       </c>
@@ -41765,8 +42051,11 @@
       <c r="L37">
         <v>-92.196700000000007</v>
       </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M37" s="84">
+        <v>4.3332229386391701</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>232</v>
       </c>
@@ -41798,7 +42087,7 @@
         <v>-92.196700000000007</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>232</v>
       </c>
@@ -41830,7 +42119,7 @@
         <v>-92.196700000000007</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>232</v>
       </c>
@@ -41862,7 +42151,7 @@
         <v>-92.196700000000007</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>232</v>
       </c>
@@ -41894,7 +42183,7 @@
         <v>-92.196700000000007</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>232</v>
       </c>
@@ -41926,7 +42215,7 @@
         <v>-92.196700000000007</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>232</v>
       </c>
@@ -41958,7 +42247,7 @@
         <v>-92.196700000000007</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>232</v>
       </c>
@@ -41990,7 +42279,7 @@
         <v>-92.196700000000007</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>232</v>
       </c>
@@ -42022,7 +42311,7 @@
         <v>-92.196700000000007</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>232</v>
       </c>
@@ -42054,7 +42343,7 @@
         <v>-92.196700000000007</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>232</v>
       </c>
@@ -42086,7 +42375,7 @@
         <v>-92.196700000000007</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>232</v>
       </c>
@@ -67353,20 +67642,26 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AJ47"/>
+  <dimension ref="A1:AJ107"/>
   <sheetViews>
     <sheetView zoomScale="101" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E6"/>
+      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G35" sqref="G35:K35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.85546875" style="15" customWidth="1"/>
+    <col min="1" max="1" width="7.42578125" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" style="15" customWidth="1"/>
     <col min="4" max="4" width="22.85546875" style="15" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="24.5703125" style="15" customWidth="1"/>
-    <col min="6" max="7" width="9.140625" style="60"/>
-    <col min="8" max="8" width="14.28515625" style="60" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" style="15" customWidth="1"/>
+    <col min="6" max="7" width="12.5703125" style="60" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" style="60" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.7109375" style="17" customWidth="1"/>
+    <col min="11" max="11" width="12.5703125" style="17" bestFit="1" customWidth="1"/>
+    <col min="12" max="16" width="12" style="17" bestFit="1" customWidth="1"/>
     <col min="19" max="25" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="27" max="30" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="13.140625" bestFit="1" customWidth="1"/>
@@ -67375,7 +67670,7 @@
     <col min="36" max="36" width="19.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:36" ht="90" x14ac:dyDescent="0.25">
       <c r="A1" s="58" t="s">
         <v>217</v>
       </c>
@@ -67394,6 +67689,27 @@
       <c r="F1" s="59"/>
       <c r="G1" s="59"/>
       <c r="H1" s="59"/>
+      <c r="J1" s="17" t="s">
+        <v>440</v>
+      </c>
+      <c r="K1" s="17" t="s">
+        <v>441</v>
+      </c>
+      <c r="L1" s="79" t="s">
+        <v>442</v>
+      </c>
+      <c r="M1" s="79" t="s">
+        <v>443</v>
+      </c>
+      <c r="N1" s="79" t="s">
+        <v>444</v>
+      </c>
+      <c r="O1" s="80" t="s">
+        <v>445</v>
+      </c>
+      <c r="P1" s="80" t="s">
+        <v>446</v>
+      </c>
       <c r="T1">
         <v>1</v>
       </c>
@@ -67454,6 +67770,27 @@
         <f t="shared" ref="H2:H31" si="0">(E2-C2)/E2</f>
         <v>-1.570343343829357</v>
       </c>
+      <c r="J2" s="17">
+        <v>2007</v>
+      </c>
+      <c r="K2" s="17">
+        <v>32.525867683855601</v>
+      </c>
+      <c r="L2" s="79">
+        <v>43.715831081228103</v>
+      </c>
+      <c r="M2" s="79">
+        <v>19.095838707493002</v>
+      </c>
+      <c r="N2" s="79">
+        <v>27.370114686652201</v>
+      </c>
+      <c r="O2" s="80">
+        <v>37.154797204354303</v>
+      </c>
+      <c r="P2" s="80">
+        <v>19.512016956402899</v>
+      </c>
       <c r="S2">
         <v>2011</v>
       </c>
@@ -67527,6 +67864,27 @@
         <f t="shared" si="0"/>
         <v>0.22770471634197734</v>
       </c>
+      <c r="J3" s="17">
+        <v>2008</v>
+      </c>
+      <c r="K3" s="17">
+        <v>23.058711672222199</v>
+      </c>
+      <c r="L3" s="79">
+        <v>25.886014461666701</v>
+      </c>
+      <c r="M3" s="79">
+        <v>21.198533416210001</v>
+      </c>
+      <c r="N3" s="79">
+        <v>22.3685433553586</v>
+      </c>
+      <c r="O3" s="80">
+        <v>22.991812047709999</v>
+      </c>
+      <c r="P3" s="80">
+        <v>18.1524880755853</v>
+      </c>
       <c r="S3">
         <v>2012</v>
       </c>
@@ -67601,6 +67959,27 @@
         <f t="shared" si="0"/>
         <v>0.13596782836876695</v>
       </c>
+      <c r="J4" s="17">
+        <v>2009</v>
+      </c>
+      <c r="K4" s="17">
+        <v>31.0960956387378</v>
+      </c>
+      <c r="L4" s="79">
+        <v>0</v>
+      </c>
+      <c r="M4" s="79">
+        <v>14.33156483408</v>
+      </c>
+      <c r="N4" s="79">
+        <v>24.972719571799999</v>
+      </c>
+      <c r="O4" s="80">
+        <v>47.726308199400002</v>
+      </c>
+      <c r="P4" s="80">
+        <v>19.0556452217537</v>
+      </c>
       <c r="S4">
         <v>2013</v>
       </c>
@@ -67675,6 +68054,27 @@
         <f t="shared" si="0"/>
         <v>0.40645420586368719</v>
       </c>
+      <c r="J5" s="17">
+        <v>2010</v>
+      </c>
+      <c r="K5" s="17">
+        <v>28.144987626739901</v>
+      </c>
+      <c r="L5" s="79">
+        <v>0</v>
+      </c>
+      <c r="M5" s="79">
+        <v>17.389732712366701</v>
+      </c>
+      <c r="N5" s="79">
+        <v>21.8253746110333</v>
+      </c>
+      <c r="O5" s="80">
+        <v>29.455664928803898</v>
+      </c>
+      <c r="P5" s="80">
+        <v>21.009354907007499</v>
+      </c>
       <c r="S5">
         <v>2014</v>
       </c>
@@ -67749,6 +68149,27 @@
         <f t="shared" si="0"/>
         <v>0.38960230835600357</v>
       </c>
+      <c r="J6" s="17">
+        <v>2011</v>
+      </c>
+      <c r="K6" s="17">
+        <v>9.1025996493385506</v>
+      </c>
+      <c r="L6" s="79">
+        <v>30.2445924049733</v>
+      </c>
+      <c r="M6" s="79">
+        <v>9.7001828208000003</v>
+      </c>
+      <c r="N6" s="79">
+        <v>9.5913074339377609</v>
+      </c>
+      <c r="O6" s="80">
+        <v>19.05049434675</v>
+      </c>
+      <c r="P6" s="80">
+        <v>5.5771901070694296</v>
+      </c>
       <c r="S6">
         <v>2015</v>
       </c>
@@ -67823,6 +68244,27 @@
         <f t="shared" si="0"/>
         <v>-1.7851572277004391E-3</v>
       </c>
+      <c r="J7" s="17">
+        <v>2012</v>
+      </c>
+      <c r="K7" s="17">
+        <v>14.461191714423901</v>
+      </c>
+      <c r="L7" s="79">
+        <v>12.322867652470499</v>
+      </c>
+      <c r="M7" s="79">
+        <v>4.2925759112617303</v>
+      </c>
+      <c r="N7" s="79">
+        <v>5.9977010626825402</v>
+      </c>
+      <c r="O7" s="80">
+        <v>7.7289606995984901</v>
+      </c>
+      <c r="P7" s="80">
+        <v>3.6994482564836701</v>
+      </c>
       <c r="AA7" s="42">
         <v>1</v>
       </c>
@@ -67874,6 +68316,27 @@
         <f t="shared" si="0"/>
         <v>-1.7864169227517488E-3</v>
       </c>
+      <c r="J8" s="17">
+        <v>2013</v>
+      </c>
+      <c r="K8" s="17">
+        <v>23.8985946874608</v>
+      </c>
+      <c r="L8" s="79">
+        <v>32.235161800374001</v>
+      </c>
+      <c r="M8" s="79">
+        <v>19.1132729249378</v>
+      </c>
+      <c r="N8" s="79">
+        <v>20.819684091088099</v>
+      </c>
+      <c r="O8" s="80">
+        <v>36.226840773504399</v>
+      </c>
+      <c r="P8" s="80">
+        <v>16.271459630304602</v>
+      </c>
       <c r="T8">
         <v>2011</v>
       </c>
@@ -67942,6 +68405,27 @@
         <f t="shared" si="0"/>
         <v>-1.7863049230554503E-3</v>
       </c>
+      <c r="J9" s="17">
+        <v>2014</v>
+      </c>
+      <c r="K9" s="17">
+        <v>37.154274293639098</v>
+      </c>
+      <c r="L9" s="79">
+        <v>59.172386135875797</v>
+      </c>
+      <c r="M9" s="79">
+        <v>6.4707712039542704</v>
+      </c>
+      <c r="N9" s="79">
+        <v>15.6447669866408</v>
+      </c>
+      <c r="O9" s="80">
+        <v>56.005994075571202</v>
+      </c>
+      <c r="P9" s="80">
+        <v>13.224573919535301</v>
+      </c>
       <c r="S9">
         <v>1</v>
       </c>
@@ -68001,6 +68485,27 @@
         <f t="shared" si="0"/>
         <v>-1.7860975121028E-3</v>
       </c>
+      <c r="J10" s="17">
+        <v>2015</v>
+      </c>
+      <c r="K10" s="17">
+        <v>10.6238939286857</v>
+      </c>
+      <c r="L10" s="79">
+        <v>14.9004345219195</v>
+      </c>
+      <c r="M10" s="79">
+        <v>10.6102212874851</v>
+      </c>
+      <c r="N10" s="79">
+        <v>9.9696464002593608</v>
+      </c>
+      <c r="O10" s="80">
+        <v>51.166072198054799</v>
+      </c>
+      <c r="P10" s="80">
+        <v>23.589501119907499</v>
+      </c>
       <c r="S10">
         <v>2</v>
       </c>
@@ -68060,6 +68565,27 @@
         <f t="shared" si="0"/>
         <v>-1.7861345131077145E-3</v>
       </c>
+      <c r="J11" s="17">
+        <v>2016</v>
+      </c>
+      <c r="K11" s="17">
+        <v>9.3818217310323497</v>
+      </c>
+      <c r="L11" s="79">
+        <v>14.7041876082792</v>
+      </c>
+      <c r="M11" s="79">
+        <v>3.3268933406616301</v>
+      </c>
+      <c r="N11" s="79">
+        <v>1.3664545382970901</v>
+      </c>
+      <c r="O11" s="80">
+        <v>20.138381222186901</v>
+      </c>
+      <c r="P11" s="80">
+        <v>4.3332229386391701</v>
+      </c>
       <c r="S11">
         <v>3</v>
       </c>
@@ -68119,6 +68645,11 @@
         <f t="shared" si="0"/>
         <v>-1.7862331148862398E-3</v>
       </c>
+      <c r="L12" s="79"/>
+      <c r="M12" s="79"/>
+      <c r="N12" s="79"/>
+      <c r="O12" s="80"/>
+      <c r="P12" s="80"/>
       <c r="S12">
         <v>4</v>
       </c>
@@ -68176,6 +68707,11 @@
         <f t="shared" si="0"/>
         <v>-1.7860443493506375E-3</v>
       </c>
+      <c r="L13" s="79"/>
+      <c r="M13" s="79"/>
+      <c r="N13" s="79"/>
+      <c r="O13" s="80"/>
+      <c r="P13" s="80"/>
       <c r="S13">
         <v>5</v>
       </c>
@@ -68235,6 +68771,11 @@
         <f t="shared" si="0"/>
         <v>-1.7864323834320156E-3</v>
       </c>
+      <c r="L14" s="79"/>
+      <c r="M14" s="79"/>
+      <c r="N14" s="79"/>
+      <c r="O14" s="80"/>
+      <c r="P14" s="80"/>
       <c r="S14">
         <v>6</v>
       </c>
@@ -68294,6 +68835,11 @@
         <f t="shared" si="0"/>
         <v>-1.7861330615513845E-3</v>
       </c>
+      <c r="L15" s="79"/>
+      <c r="M15" s="79"/>
+      <c r="N15" s="79"/>
+      <c r="O15" s="80"/>
+      <c r="P15" s="80"/>
       <c r="AA15" s="1">
         <v>3</v>
       </c>
@@ -68335,6 +68881,11 @@
         <f t="shared" si="0"/>
         <v>-1.7864325925982215E-3</v>
       </c>
+      <c r="L16" s="79"/>
+      <c r="M16" s="79"/>
+      <c r="N16" s="79"/>
+      <c r="O16" s="80"/>
+      <c r="P16" s="80"/>
       <c r="S16" s="77" t="s">
         <v>49</v>
       </c>
@@ -68387,6 +68938,11 @@
         <f t="shared" si="0"/>
         <v>-1.7862775505954004E-3</v>
       </c>
+      <c r="L17" s="79"/>
+      <c r="M17" s="79"/>
+      <c r="N17" s="79"/>
+      <c r="O17" s="80"/>
+      <c r="P17" s="80"/>
       <c r="S17" s="78"/>
       <c r="T17" s="78"/>
       <c r="U17" s="44" t="s">
@@ -68437,6 +68993,11 @@
         <f t="shared" si="0"/>
         <v>-1.7862013523618698E-3</v>
       </c>
+      <c r="L18" s="79"/>
+      <c r="M18" s="79"/>
+      <c r="N18" s="79"/>
+      <c r="O18" s="80"/>
+      <c r="P18" s="80"/>
       <c r="S18" s="1">
         <v>1</v>
       </c>
@@ -68494,6 +69055,11 @@
         <f t="shared" si="0"/>
         <v>-1.7862067471861674E-3</v>
       </c>
+      <c r="L19" s="79"/>
+      <c r="M19" s="79"/>
+      <c r="N19" s="79"/>
+      <c r="O19" s="80"/>
+      <c r="P19" s="80"/>
       <c r="S19" s="1">
         <v>2</v>
       </c>
@@ -68551,6 +69117,11 @@
         <f t="shared" si="0"/>
         <v>-1.7864061477670592E-3</v>
       </c>
+      <c r="L20" s="79"/>
+      <c r="M20" s="79"/>
+      <c r="N20" s="79"/>
+      <c r="O20" s="80"/>
+      <c r="P20" s="80"/>
       <c r="S20" s="1">
         <v>3</v>
       </c>
@@ -68611,6 +69182,11 @@
         <f t="shared" si="0"/>
         <v>-1.7861987608346148E-3</v>
       </c>
+      <c r="L21" s="79"/>
+      <c r="M21" s="79"/>
+      <c r="N21" s="79"/>
+      <c r="O21" s="80"/>
+      <c r="P21" s="80"/>
       <c r="S21" s="1">
         <v>4</v>
       </c>
@@ -68668,6 +69244,11 @@
         <f t="shared" si="0"/>
         <v>-1.7859491099447981E-3</v>
       </c>
+      <c r="L22" s="79"/>
+      <c r="M22" s="79"/>
+      <c r="N22" s="79"/>
+      <c r="O22" s="80"/>
+      <c r="P22" s="80"/>
       <c r="S22" s="1">
         <v>5</v>
       </c>
@@ -68723,6 +69304,11 @@
         <f t="shared" si="0"/>
         <v>-152681.14136708158</v>
       </c>
+      <c r="L23" s="79"/>
+      <c r="M23" s="79"/>
+      <c r="N23" s="79"/>
+      <c r="O23" s="80"/>
+      <c r="P23" s="80"/>
       <c r="S23" s="1">
         <v>6</v>
       </c>
@@ -68780,6 +69366,11 @@
         <f t="shared" si="0"/>
         <v>-1.7860694494352838E-3</v>
       </c>
+      <c r="L24" s="79"/>
+      <c r="M24" s="79"/>
+      <c r="N24" s="79"/>
+      <c r="O24" s="80"/>
+      <c r="P24" s="80"/>
       <c r="S24" s="1">
         <v>1</v>
       </c>
@@ -68837,6 +69428,11 @@
         <f t="shared" si="0"/>
         <v>-1.7861933551667386E-3</v>
       </c>
+      <c r="L25" s="79"/>
+      <c r="M25" s="79"/>
+      <c r="N25" s="79"/>
+      <c r="O25" s="80"/>
+      <c r="P25" s="80"/>
       <c r="S25" s="1">
         <v>2</v>
       </c>
@@ -68894,6 +69490,11 @@
         <f t="shared" si="0"/>
         <v>-1.78620178314674E-3</v>
       </c>
+      <c r="L26" s="79"/>
+      <c r="M26" s="79"/>
+      <c r="N26" s="79"/>
+      <c r="O26" s="80"/>
+      <c r="P26" s="80"/>
       <c r="S26" s="1">
         <v>3</v>
       </c>
@@ -68951,6 +69552,11 @@
         <f t="shared" si="0"/>
         <v>-1.7863423217456852E-3</v>
       </c>
+      <c r="L27" s="79"/>
+      <c r="M27" s="79"/>
+      <c r="N27" s="79"/>
+      <c r="O27" s="80"/>
+      <c r="P27" s="80"/>
       <c r="S27" s="1">
         <v>4</v>
       </c>
@@ -69006,6 +69612,11 @@
         <f t="shared" si="0"/>
         <v>-1.7861533578925034E-3</v>
       </c>
+      <c r="L28" s="79"/>
+      <c r="M28" s="79"/>
+      <c r="N28" s="79"/>
+      <c r="O28" s="80"/>
+      <c r="P28" s="80"/>
       <c r="S28" s="1">
         <v>5</v>
       </c>
@@ -69063,6 +69674,11 @@
         <f t="shared" si="0"/>
         <v>-1.7863696033928237E-3</v>
       </c>
+      <c r="L29" s="79"/>
+      <c r="M29" s="79"/>
+      <c r="N29" s="79"/>
+      <c r="O29" s="80"/>
+      <c r="P29" s="80"/>
       <c r="S29" s="1">
         <v>6</v>
       </c>
@@ -69120,6 +69736,11 @@
         <f t="shared" si="0"/>
         <v>-1.7859716459460357E-3</v>
       </c>
+      <c r="L30" s="79"/>
+      <c r="M30" s="79"/>
+      <c r="N30" s="79"/>
+      <c r="O30" s="80"/>
+      <c r="P30" s="80"/>
       <c r="S30" s="1">
         <v>1</v>
       </c>
@@ -69177,6 +69798,11 @@
         <f t="shared" si="0"/>
         <v>-1.7863680184829495E-3</v>
       </c>
+      <c r="L31" s="79"/>
+      <c r="M31" s="79"/>
+      <c r="N31" s="79"/>
+      <c r="O31" s="80"/>
+      <c r="P31" s="80"/>
       <c r="S31" s="1">
         <v>2</v>
       </c>
@@ -69211,6 +69837,11 @@
       </c>
     </row>
     <row r="32" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="L32" s="79"/>
+      <c r="M32" s="79"/>
+      <c r="N32" s="79"/>
+      <c r="O32" s="80"/>
+      <c r="P32" s="80"/>
       <c r="S32" s="1">
         <v>3</v>
       </c>
@@ -69242,7 +69873,12 @@
         <v>23.588162023184807</v>
       </c>
     </row>
-    <row r="33" spans="19:24" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="L33" s="79"/>
+      <c r="M33" s="79"/>
+      <c r="N33" s="79"/>
+      <c r="O33" s="80"/>
+      <c r="P33" s="80"/>
       <c r="S33" s="1">
         <v>4</v>
       </c>
@@ -69260,7 +69896,12 @@
         <v>0.69922129383209608</v>
       </c>
     </row>
-    <row r="34" spans="19:24" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="L34" s="79"/>
+      <c r="M34" s="79"/>
+      <c r="N34" s="79"/>
+      <c r="O34" s="80"/>
+      <c r="P34" s="80"/>
       <c r="S34" s="1">
         <v>5</v>
       </c>
@@ -69278,7 +69919,35 @@
         <v>0.80993384737238472</v>
       </c>
     </row>
-    <row r="35" spans="19:24" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A35" s="81" t="s">
+        <v>440</v>
+      </c>
+      <c r="B35" s="81">
+        <v>2007</v>
+      </c>
+      <c r="C35" s="81">
+        <v>2008</v>
+      </c>
+      <c r="D35" s="81">
+        <v>2009</v>
+      </c>
+      <c r="E35" s="81">
+        <v>2010</v>
+      </c>
+      <c r="F35" s="81">
+        <v>2011</v>
+      </c>
+      <c r="G35" s="81"/>
+      <c r="H35" s="81"/>
+      <c r="I35" s="81"/>
+      <c r="J35" s="81"/>
+      <c r="K35" s="81"/>
+      <c r="L35" s="79"/>
+      <c r="M35" s="79"/>
+      <c r="N35" s="79"/>
+      <c r="O35" s="80"/>
+      <c r="P35" s="80"/>
       <c r="S35" s="1">
         <v>6</v>
       </c>
@@ -69296,7 +69965,30 @@
         <v>0.32675268400698876</v>
       </c>
     </row>
-    <row r="36" spans="19:24" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A36" s="81" t="s">
+        <v>441</v>
+      </c>
+      <c r="B36" s="83">
+        <v>32.525867683855601</v>
+      </c>
+      <c r="C36" s="83">
+        <v>23.058711672222199</v>
+      </c>
+      <c r="D36" s="83">
+        <v>31.0960956387378</v>
+      </c>
+      <c r="E36" s="83">
+        <v>28.144987626739901</v>
+      </c>
+      <c r="F36" s="83">
+        <v>9.1025996493385506</v>
+      </c>
+      <c r="L36" s="79"/>
+      <c r="M36" s="79"/>
+      <c r="N36" s="79"/>
+      <c r="O36" s="80"/>
+      <c r="P36" s="80"/>
       <c r="S36" s="1">
         <v>1</v>
       </c>
@@ -69314,7 +70006,30 @@
         <v>-8.2850647939563586</v>
       </c>
     </row>
-    <row r="37" spans="19:24" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A37" s="81" t="s">
+        <v>442</v>
+      </c>
+      <c r="B37" s="83">
+        <v>43.715831081228103</v>
+      </c>
+      <c r="C37" s="83">
+        <v>25.886014461666701</v>
+      </c>
+      <c r="D37" s="83">
+        <v>0</v>
+      </c>
+      <c r="E37" s="83">
+        <v>0</v>
+      </c>
+      <c r="F37" s="83">
+        <v>30.2445924049733</v>
+      </c>
+      <c r="L37" s="79"/>
+      <c r="M37" s="79"/>
+      <c r="N37" s="79"/>
+      <c r="O37" s="80"/>
+      <c r="P37" s="80"/>
       <c r="S37" s="1">
         <v>2</v>
       </c>
@@ -69332,7 +70047,30 @@
         <v>2.3004960969402646</v>
       </c>
     </row>
-    <row r="38" spans="19:24" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A38" s="81" t="s">
+        <v>443</v>
+      </c>
+      <c r="B38" s="83">
+        <v>19.095838707493002</v>
+      </c>
+      <c r="C38" s="83">
+        <v>21.198533416210001</v>
+      </c>
+      <c r="D38" s="83">
+        <v>14.33156483408</v>
+      </c>
+      <c r="E38" s="83">
+        <v>17.389732712366701</v>
+      </c>
+      <c r="F38" s="83">
+        <v>9.7001828208000003</v>
+      </c>
+      <c r="L38" s="79"/>
+      <c r="M38" s="79"/>
+      <c r="N38" s="79"/>
+      <c r="O38" s="80"/>
+      <c r="P38" s="80"/>
       <c r="S38" s="1">
         <v>3</v>
       </c>
@@ -69350,7 +70088,30 @@
         <v>-10.067110011531941</v>
       </c>
     </row>
-    <row r="39" spans="19:24" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A39" s="81" t="s">
+        <v>444</v>
+      </c>
+      <c r="B39" s="83">
+        <v>27.370114686652201</v>
+      </c>
+      <c r="C39" s="83">
+        <v>22.3685433553586</v>
+      </c>
+      <c r="D39" s="83">
+        <v>24.972719571799999</v>
+      </c>
+      <c r="E39" s="83">
+        <v>21.8253746110333</v>
+      </c>
+      <c r="F39" s="83">
+        <v>9.5913074339377609</v>
+      </c>
+      <c r="L39" s="79"/>
+      <c r="M39" s="79"/>
+      <c r="N39" s="79"/>
+      <c r="O39" s="80"/>
+      <c r="P39" s="80"/>
       <c r="S39" s="1">
         <v>4</v>
       </c>
@@ -69368,7 +70129,30 @@
         <v>4.973132320845508E-2</v>
       </c>
     </row>
-    <row r="40" spans="19:24" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A40" s="82" t="s">
+        <v>445</v>
+      </c>
+      <c r="B40" s="84">
+        <v>37.154797204354303</v>
+      </c>
+      <c r="C40" s="84">
+        <v>22.991812047709999</v>
+      </c>
+      <c r="D40" s="84">
+        <v>47.726308199400002</v>
+      </c>
+      <c r="E40" s="84">
+        <v>29.455664928803898</v>
+      </c>
+      <c r="F40" s="84">
+        <v>19.05049434675</v>
+      </c>
+      <c r="L40" s="79"/>
+      <c r="M40" s="79"/>
+      <c r="N40" s="79"/>
+      <c r="O40" s="80"/>
+      <c r="P40" s="80"/>
       <c r="S40" s="1">
         <v>5</v>
       </c>
@@ -69386,7 +70170,30 @@
         <v>0.11806283013723373</v>
       </c>
     </row>
-    <row r="41" spans="19:24" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A41" s="82" t="s">
+        <v>446</v>
+      </c>
+      <c r="B41" s="84">
+        <v>19.512016956402899</v>
+      </c>
+      <c r="C41" s="84">
+        <v>18.1524880755853</v>
+      </c>
+      <c r="D41" s="84">
+        <v>19.0556452217537</v>
+      </c>
+      <c r="E41" s="84">
+        <v>21.009354907007499</v>
+      </c>
+      <c r="F41" s="84">
+        <v>5.5771901070694296</v>
+      </c>
+      <c r="L41" s="79"/>
+      <c r="M41" s="79"/>
+      <c r="N41" s="79"/>
+      <c r="O41" s="80"/>
+      <c r="P41" s="80"/>
       <c r="S41" s="1">
         <v>6</v>
       </c>
@@ -69404,7 +70211,15 @@
         <v>1.4589059353748777</v>
       </c>
     </row>
-    <row r="42" spans="19:24" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="F42" s="83">
+        <v>14.461191714423901</v>
+      </c>
+      <c r="L42" s="79"/>
+      <c r="M42" s="79"/>
+      <c r="N42" s="79"/>
+      <c r="O42" s="80"/>
+      <c r="P42" s="80"/>
       <c r="S42" s="42">
         <v>1</v>
       </c>
@@ -69420,7 +70235,15 @@
         <v>6.4732370062486293</v>
       </c>
     </row>
-    <row r="43" spans="19:24" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="F43" s="83">
+        <v>12.322867652470499</v>
+      </c>
+      <c r="L43" s="79"/>
+      <c r="M43" s="79"/>
+      <c r="N43" s="79"/>
+      <c r="O43" s="80"/>
+      <c r="P43" s="80"/>
       <c r="S43" s="1">
         <v>2</v>
       </c>
@@ -69436,7 +70259,15 @@
         <v>14.899464757295986</v>
       </c>
     </row>
-    <row r="44" spans="19:24" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="F44" s="83">
+        <v>4.2925759112617303</v>
+      </c>
+      <c r="L44" s="79"/>
+      <c r="M44" s="79"/>
+      <c r="N44" s="79"/>
+      <c r="O44" s="80"/>
+      <c r="P44" s="80"/>
       <c r="S44" s="1">
         <v>3</v>
       </c>
@@ -69452,7 +70283,15 @@
         <v>10.609299296662067</v>
       </c>
     </row>
-    <row r="45" spans="19:24" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="F45" s="83">
+        <v>5.9977010626825402</v>
+      </c>
+      <c r="L45" s="79"/>
+      <c r="M45" s="79"/>
+      <c r="N45" s="79"/>
+      <c r="O45" s="80"/>
+      <c r="P45" s="80"/>
       <c r="S45" s="1">
         <v>4</v>
       </c>
@@ -69471,7 +70310,15 @@
         <v>9.9700000000000006</v>
       </c>
     </row>
-    <row r="46" spans="19:24" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="F46" s="84">
+        <v>7.7289606995984901</v>
+      </c>
+      <c r="L46" s="79"/>
+      <c r="M46" s="79"/>
+      <c r="N46" s="79"/>
+      <c r="O46" s="80"/>
+      <c r="P46" s="80"/>
       <c r="S46" s="1">
         <v>5</v>
       </c>
@@ -69487,7 +70334,15 @@
         <v>51.15374766070407</v>
       </c>
     </row>
-    <row r="47" spans="19:24" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="F47" s="84">
+        <v>3.6994482564836701</v>
+      </c>
+      <c r="L47" s="79"/>
+      <c r="M47" s="79"/>
+      <c r="N47" s="79"/>
+      <c r="O47" s="80"/>
+      <c r="P47" s="80"/>
       <c r="S47" s="42">
         <v>6</v>
       </c>
@@ -69502,6 +70357,498 @@
         <f t="shared" si="2"/>
         <v>23.588162023184807</v>
       </c>
+    </row>
+    <row r="48" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="F48" s="83">
+        <v>23.8985946874608</v>
+      </c>
+      <c r="L48" s="79"/>
+      <c r="M48" s="79"/>
+      <c r="N48" s="79"/>
+      <c r="O48" s="80"/>
+      <c r="P48" s="80"/>
+    </row>
+    <row r="49" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F49" s="83">
+        <v>32.235161800374001</v>
+      </c>
+      <c r="L49" s="79"/>
+      <c r="M49" s="79"/>
+      <c r="N49" s="79"/>
+      <c r="O49" s="80"/>
+      <c r="P49" s="80"/>
+    </row>
+    <row r="50" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F50" s="83">
+        <v>19.1132729249378</v>
+      </c>
+      <c r="L50" s="79"/>
+      <c r="M50" s="79"/>
+      <c r="N50" s="79"/>
+      <c r="O50" s="80"/>
+      <c r="P50" s="80"/>
+    </row>
+    <row r="51" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F51" s="83">
+        <v>20.819684091088099</v>
+      </c>
+      <c r="L51" s="79"/>
+      <c r="M51" s="79"/>
+      <c r="N51" s="79"/>
+      <c r="O51" s="80"/>
+      <c r="P51" s="80"/>
+    </row>
+    <row r="52" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F52" s="84">
+        <v>36.226840773504399</v>
+      </c>
+      <c r="L52" s="79"/>
+      <c r="M52" s="79"/>
+      <c r="N52" s="79"/>
+      <c r="O52" s="80"/>
+      <c r="P52" s="80"/>
+    </row>
+    <row r="53" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F53" s="84">
+        <v>16.271459630304602</v>
+      </c>
+      <c r="L53" s="79"/>
+      <c r="M53" s="79"/>
+      <c r="N53" s="79"/>
+      <c r="O53" s="80"/>
+      <c r="P53" s="80"/>
+    </row>
+    <row r="54" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F54" s="83">
+        <v>37.154274293639098</v>
+      </c>
+      <c r="L54" s="79"/>
+      <c r="M54" s="79"/>
+      <c r="N54" s="79"/>
+      <c r="O54" s="80"/>
+      <c r="P54" s="80"/>
+    </row>
+    <row r="55" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F55" s="83">
+        <v>59.172386135875797</v>
+      </c>
+      <c r="L55" s="79"/>
+      <c r="M55" s="79"/>
+      <c r="N55" s="79"/>
+      <c r="O55" s="80"/>
+      <c r="P55" s="80"/>
+    </row>
+    <row r="56" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F56" s="83">
+        <v>6.4707712039542704</v>
+      </c>
+      <c r="L56" s="79"/>
+      <c r="M56" s="79"/>
+      <c r="N56" s="79"/>
+      <c r="O56" s="80"/>
+      <c r="P56" s="80"/>
+    </row>
+    <row r="57" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F57" s="83">
+        <v>15.6447669866408</v>
+      </c>
+      <c r="L57" s="79"/>
+      <c r="M57" s="79"/>
+      <c r="N57" s="79"/>
+      <c r="O57" s="80"/>
+      <c r="P57" s="80"/>
+    </row>
+    <row r="58" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F58" s="84">
+        <v>56.005994075571202</v>
+      </c>
+      <c r="L58" s="79"/>
+      <c r="M58" s="79"/>
+      <c r="N58" s="79"/>
+      <c r="O58" s="80"/>
+      <c r="P58" s="80"/>
+    </row>
+    <row r="59" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F59" s="84">
+        <v>13.224573919535301</v>
+      </c>
+      <c r="L59" s="79"/>
+      <c r="M59" s="79"/>
+      <c r="N59" s="79"/>
+      <c r="O59" s="80"/>
+      <c r="P59" s="80"/>
+    </row>
+    <row r="60" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F60" s="83">
+        <v>10.6238939286857</v>
+      </c>
+      <c r="L60" s="79"/>
+      <c r="M60" s="79"/>
+      <c r="N60" s="79"/>
+      <c r="O60" s="80"/>
+      <c r="P60" s="80"/>
+    </row>
+    <row r="61" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F61" s="83">
+        <v>14.9004345219195</v>
+      </c>
+      <c r="L61" s="79"/>
+      <c r="M61" s="79"/>
+      <c r="N61" s="79"/>
+      <c r="O61" s="80"/>
+      <c r="P61" s="80"/>
+    </row>
+    <row r="62" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F62" s="83">
+        <v>10.6102212874851</v>
+      </c>
+      <c r="L62" s="79"/>
+      <c r="M62" s="79"/>
+      <c r="N62" s="79"/>
+      <c r="O62" s="80"/>
+      <c r="P62" s="80"/>
+    </row>
+    <row r="63" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F63" s="83">
+        <v>9.9696464002593608</v>
+      </c>
+      <c r="L63" s="79"/>
+      <c r="M63" s="79"/>
+      <c r="N63" s="79"/>
+      <c r="O63" s="80"/>
+      <c r="P63" s="80"/>
+    </row>
+    <row r="64" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F64" s="84">
+        <v>51.166072198054799</v>
+      </c>
+      <c r="L64" s="79"/>
+      <c r="M64" s="79"/>
+      <c r="N64" s="79"/>
+      <c r="O64" s="80"/>
+      <c r="P64" s="80"/>
+    </row>
+    <row r="65" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F65" s="84">
+        <v>23.589501119907499</v>
+      </c>
+      <c r="L65" s="79"/>
+      <c r="M65" s="79"/>
+      <c r="N65" s="79"/>
+      <c r="O65" s="80"/>
+      <c r="P65" s="80"/>
+    </row>
+    <row r="66" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F66" s="83">
+        <v>9.3818217310323497</v>
+      </c>
+      <c r="L66" s="79"/>
+      <c r="M66" s="79"/>
+      <c r="N66" s="79"/>
+      <c r="O66" s="80"/>
+      <c r="P66" s="80"/>
+    </row>
+    <row r="67" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F67" s="83">
+        <v>14.7041876082792</v>
+      </c>
+      <c r="L67" s="79"/>
+      <c r="M67" s="79"/>
+      <c r="N67" s="79"/>
+      <c r="O67" s="80"/>
+      <c r="P67" s="80"/>
+    </row>
+    <row r="68" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F68" s="83">
+        <v>3.3268933406616301</v>
+      </c>
+      <c r="L68" s="79"/>
+      <c r="M68" s="79"/>
+      <c r="N68" s="79"/>
+      <c r="O68" s="80"/>
+      <c r="P68" s="80"/>
+    </row>
+    <row r="69" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F69" s="83">
+        <v>1.3664545382970901</v>
+      </c>
+      <c r="L69" s="79"/>
+      <c r="M69" s="79"/>
+      <c r="N69" s="79"/>
+      <c r="O69" s="80"/>
+      <c r="P69" s="80"/>
+    </row>
+    <row r="70" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F70" s="84">
+        <v>20.138381222186901</v>
+      </c>
+      <c r="L70" s="79"/>
+      <c r="M70" s="79"/>
+      <c r="N70" s="79"/>
+      <c r="O70" s="80"/>
+      <c r="P70" s="80"/>
+    </row>
+    <row r="71" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F71" s="84">
+        <v>4.3332229386391701</v>
+      </c>
+      <c r="L71" s="79"/>
+      <c r="M71" s="79"/>
+      <c r="N71" s="79"/>
+      <c r="O71" s="80"/>
+      <c r="P71" s="80"/>
+    </row>
+    <row r="72" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="L72" s="79"/>
+      <c r="M72" s="79"/>
+      <c r="N72" s="79"/>
+      <c r="O72" s="80"/>
+      <c r="P72" s="80"/>
+    </row>
+    <row r="73" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="L73" s="79"/>
+      <c r="M73" s="79"/>
+      <c r="N73" s="79"/>
+      <c r="O73" s="80"/>
+      <c r="P73" s="80"/>
+    </row>
+    <row r="74" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="L74" s="79"/>
+      <c r="M74" s="79"/>
+      <c r="N74" s="79"/>
+      <c r="O74" s="80"/>
+      <c r="P74" s="80"/>
+    </row>
+    <row r="75" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="L75" s="79"/>
+      <c r="M75" s="79"/>
+      <c r="N75" s="79"/>
+      <c r="O75" s="80"/>
+      <c r="P75" s="80"/>
+    </row>
+    <row r="76" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="L76" s="79"/>
+      <c r="M76" s="79"/>
+      <c r="N76" s="79"/>
+      <c r="O76" s="80"/>
+      <c r="P76" s="80"/>
+    </row>
+    <row r="77" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="L77" s="79"/>
+      <c r="M77" s="79"/>
+      <c r="N77" s="79"/>
+      <c r="O77" s="80"/>
+      <c r="P77" s="80"/>
+    </row>
+    <row r="78" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="L78" s="79"/>
+      <c r="M78" s="79"/>
+      <c r="N78" s="79"/>
+      <c r="O78" s="80"/>
+      <c r="P78" s="80"/>
+    </row>
+    <row r="79" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="L79" s="79"/>
+      <c r="M79" s="79"/>
+      <c r="N79" s="79"/>
+      <c r="O79" s="80"/>
+      <c r="P79" s="80"/>
+    </row>
+    <row r="80" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="L80" s="79"/>
+      <c r="M80" s="79"/>
+      <c r="N80" s="79"/>
+      <c r="O80" s="80"/>
+      <c r="P80" s="80"/>
+    </row>
+    <row r="81" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="L81" s="79"/>
+      <c r="M81" s="79"/>
+      <c r="N81" s="79"/>
+      <c r="O81" s="80"/>
+      <c r="P81" s="80"/>
+    </row>
+    <row r="82" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="L82" s="79"/>
+      <c r="M82" s="79"/>
+      <c r="N82" s="79"/>
+      <c r="O82" s="80"/>
+      <c r="P82" s="80"/>
+    </row>
+    <row r="83" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="L83" s="79"/>
+      <c r="M83" s="79"/>
+      <c r="N83" s="79"/>
+      <c r="O83" s="80"/>
+      <c r="P83" s="80"/>
+    </row>
+    <row r="84" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="L84" s="79"/>
+      <c r="M84" s="79"/>
+      <c r="N84" s="79"/>
+      <c r="O84" s="80"/>
+      <c r="P84" s="80"/>
+    </row>
+    <row r="85" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="L85" s="79"/>
+      <c r="M85" s="79"/>
+      <c r="N85" s="79"/>
+      <c r="O85" s="80"/>
+      <c r="P85" s="80"/>
+    </row>
+    <row r="86" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="L86" s="79"/>
+      <c r="M86" s="79"/>
+      <c r="N86" s="79"/>
+      <c r="O86" s="80"/>
+      <c r="P86" s="80"/>
+    </row>
+    <row r="87" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="L87" s="79"/>
+      <c r="M87" s="79"/>
+      <c r="N87" s="79"/>
+      <c r="O87" s="80"/>
+      <c r="P87" s="80"/>
+    </row>
+    <row r="88" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="L88" s="79"/>
+      <c r="M88" s="79"/>
+      <c r="N88" s="79"/>
+      <c r="O88" s="80"/>
+      <c r="P88" s="80"/>
+    </row>
+    <row r="89" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="L89" s="79"/>
+      <c r="M89" s="79"/>
+      <c r="N89" s="79"/>
+      <c r="O89" s="80"/>
+      <c r="P89" s="80"/>
+    </row>
+    <row r="90" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="L90" s="79"/>
+      <c r="M90" s="79"/>
+      <c r="N90" s="79"/>
+      <c r="O90" s="80"/>
+      <c r="P90" s="80"/>
+    </row>
+    <row r="91" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="L91" s="79"/>
+      <c r="M91" s="79"/>
+      <c r="N91" s="79"/>
+      <c r="O91" s="80"/>
+      <c r="P91" s="80"/>
+    </row>
+    <row r="92" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="L92" s="79"/>
+      <c r="M92" s="79"/>
+      <c r="N92" s="79"/>
+      <c r="O92" s="80"/>
+      <c r="P92" s="80"/>
+    </row>
+    <row r="93" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="L93" s="79"/>
+      <c r="M93" s="79"/>
+      <c r="N93" s="79"/>
+      <c r="O93" s="80"/>
+      <c r="P93" s="80"/>
+    </row>
+    <row r="94" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="L94" s="79"/>
+      <c r="M94" s="79"/>
+      <c r="N94" s="79"/>
+      <c r="O94" s="80"/>
+      <c r="P94" s="80"/>
+    </row>
+    <row r="95" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="L95" s="79"/>
+      <c r="M95" s="79"/>
+      <c r="N95" s="79"/>
+      <c r="O95" s="80"/>
+      <c r="P95" s="80"/>
+    </row>
+    <row r="96" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="L96" s="79"/>
+      <c r="M96" s="79"/>
+      <c r="N96" s="79"/>
+      <c r="O96" s="80"/>
+      <c r="P96" s="80"/>
+    </row>
+    <row r="97" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="L97" s="79"/>
+      <c r="M97" s="79"/>
+      <c r="N97" s="79"/>
+      <c r="O97" s="80"/>
+      <c r="P97" s="80"/>
+    </row>
+    <row r="98" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="L98" s="79"/>
+      <c r="M98" s="79"/>
+      <c r="N98" s="79"/>
+      <c r="O98" s="80"/>
+      <c r="P98" s="80"/>
+    </row>
+    <row r="99" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="L99" s="79"/>
+      <c r="M99" s="79"/>
+      <c r="N99" s="79"/>
+      <c r="O99" s="80"/>
+      <c r="P99" s="80"/>
+    </row>
+    <row r="100" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="L100" s="79"/>
+      <c r="M100" s="79"/>
+      <c r="N100" s="79"/>
+      <c r="O100" s="80"/>
+      <c r="P100" s="80"/>
+    </row>
+    <row r="101" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="L101" s="79"/>
+      <c r="M101" s="79"/>
+      <c r="N101" s="79"/>
+      <c r="O101" s="80"/>
+      <c r="P101" s="80"/>
+    </row>
+    <row r="102" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="L102" s="79"/>
+      <c r="M102" s="79"/>
+      <c r="N102" s="79"/>
+      <c r="O102" s="80"/>
+      <c r="P102" s="80"/>
+    </row>
+    <row r="103" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="L103" s="79"/>
+      <c r="M103" s="79"/>
+      <c r="N103" s="79"/>
+      <c r="O103" s="80"/>
+      <c r="P103" s="80"/>
+    </row>
+    <row r="104" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="L104" s="79"/>
+      <c r="M104" s="79"/>
+      <c r="N104" s="79"/>
+      <c r="O104" s="80"/>
+      <c r="P104" s="80"/>
+    </row>
+    <row r="105" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="L105" s="79"/>
+      <c r="M105" s="79"/>
+      <c r="N105" s="79"/>
+      <c r="O105" s="80"/>
+      <c r="P105" s="80"/>
+    </row>
+    <row r="106" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="L106" s="79"/>
+      <c r="M106" s="79"/>
+      <c r="N106" s="79"/>
+      <c r="O106" s="80"/>
+      <c r="P106" s="80"/>
+    </row>
+    <row r="107" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="L107" s="79"/>
+      <c r="M107" s="79"/>
+      <c r="N107" s="79"/>
+      <c r="O107" s="80"/>
+      <c r="P107" s="80"/>
     </row>
   </sheetData>
   <autoFilter ref="S16:W47">

</xml_diff>